<commit_message>
Started to calc the Spike Power in Excel
Need to add random value to logging
</commit_message>
<xml_diff>
--- a/Resources/Spike Speed Tracker.xlsx
+++ b/Resources/Spike Speed Tracker.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B4359E-02F3-4F14-AF97-2574BA0BC8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6849D2CC-5370-451C-911A-9CE50DFD9C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
+    <workbookView xWindow="9274" yWindow="4980" windowWidth="23392" windowHeight="11957" activeTab="2" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Player" sheetId="1" r:id="rId1"/>
+    <sheet name="Skill to Value" sheetId="2" r:id="rId1"/>
+    <sheet name="Spike Power" sheetId="3" r:id="rId2"/>
+    <sheet name="Player" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>distance: 8.295987, power: 27.8139, speed pen: -0.01683367, set bonus: 0, spikeTime: 0.3033746, speed: 27.35m/s / 61.17mph</t>
   </si>
@@ -84,6 +86,42 @@
   </si>
   <si>
     <t>distance: 6.674328, power: 28.60008, speed pen: -0.01299713, set bonus: 0.05, spikeTime: 0.2250403, speed: 29.66m/s / 66.34mph</t>
+  </si>
+  <si>
+    <t>Player Skill</t>
+  </si>
+  <si>
+    <t>Skill Range</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Value Range</t>
+  </si>
+  <si>
+    <t>Skill to Value</t>
+  </si>
+  <si>
+    <t>Skill Type</t>
+  </si>
+  <si>
+    <t>Spike Power</t>
+  </si>
+  <si>
+    <t>maxVariance</t>
+  </si>
+  <si>
+    <t>athleteSkill</t>
+  </si>
+  <si>
+    <t>adjustedPower</t>
+  </si>
+  <si>
+    <t>athletePower</t>
   </si>
 </sst>
 </file>
@@ -119,8 +157,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,6 +498,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEFE102-FC79-44BA-9EBD-B5FDB4B0C5DA}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.15234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>22</v>
+      </c>
+      <c r="F3">
+        <v>31</v>
+      </c>
+      <c r="G3">
+        <f>(B3-C3)*(F3-E3)/(D3-C3)+E3</f>
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524659FA-A28B-4F0B-89E8-E890CA7CC901}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f>2+(0.1-2)*(A2/10)</f>
+        <v>0.67000000000000015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19289AF4-DE8A-4F06-880E-3024ABD8F25C}">
   <dimension ref="A1:A16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update logging for Spike Power
Will need to do for the Spike() function that includes the spikeSpeedPenalty based on the window and actual timing (this might be what I'm actually trying to monitor)
Next I will make an Excel to experiment with sliders and visuals
</commit_message>
<xml_diff>
--- a/Resources/Spike Speed Tracker.xlsx
+++ b/Resources/Spike Speed Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6849D2CC-5370-451C-911A-9CE50DFD9C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBDA781-0403-4D51-B869-A507DA25EDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9274" yWindow="4980" windowWidth="23392" windowHeight="11957" activeTab="2" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="2" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
   </bookViews>
   <sheets>
     <sheet name="Skill to Value" sheetId="2" r:id="rId1"/>
@@ -38,55 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
-  <si>
-    <t>distance: 8.295987, power: 27.8139, speed pen: -0.01683367, set bonus: 0, spikeTime: 0.3033746, speed: 27.35m/s / 61.17mph</t>
-  </si>
-  <si>
-    <t>distance: 8.972849, power: 27.70882, speed pen: -0.01942518, set bonus: 0, spikeTime: 0.3302415, speed: 27.17m/s / 60.78mph</t>
-  </si>
-  <si>
-    <t>distance: 9.537649, power: 27.42447, speed pen: -0.01458643, set bonus: 0, spikeTime: 0.3529268, speed: 27.02m/s / 60.45mph</t>
-  </si>
-  <si>
-    <t>distance: 6.611522, power: 28.16635, speed pen: -0.02223197, set bonus: 0, spikeTime: 0.2400684, speed: 27.54m/s / 61.61mph</t>
-  </si>
-  <si>
-    <t>distance: 6.546419, power: 27.92983, speed pen: -0.01793906, set bonus: 0, spikeTime: 0.2386696, speed: 27.43m/s / 61.36mph</t>
-  </si>
-  <si>
-    <t>distance: 6.516151, power: 28.08686, speed pen: -0.01673058, set bonus: 0, spikeTime: 0.2359475, speed: 27.62m/s / 61.78mph</t>
-  </si>
-  <si>
-    <t>distance: 6.670997, power: 27.49204, speed pen: -0.01588566, set bonus: 0.05, spikeTime: 0.2346471, speed: 28.43m/s / 63.60mph</t>
-  </si>
-  <si>
-    <t>distance: 10.03519, power: 27.48772, speed pen: -0.01465441, set bonus: 0.05, spikeTime: 0.3526155, speed: 28.46m/s / 63.66mph</t>
-  </si>
-  <si>
-    <t>distance: 6.640432, power: 28.51268, speed pen: -0.01860127, set bonus: 0.05, spikeTime: 0.225804, speed: 29.41m/s / 65.78mph</t>
-  </si>
-  <si>
-    <t>distance: 6.67511, power: 27.84725, speed pen: -0.01330408, set bonus: 0.05, spikeTime: 0.2312196, speed: 28.87m/s / 64.58mph</t>
-  </si>
-  <si>
-    <t>distance: 6.547095, power: 27.66244, speed pen: -0.02567003, set bonus: 0.05, spikeTime: 0.2310566, speed: 28.34m/s / 63.38mph</t>
-  </si>
-  <si>
-    <t>distance: 6.574227, power: 28.34016, speed pen: -0.02108194, set bonus: 0.05, spikeTime: 0.2254559, speed: 29.16m/s / 65.23mph</t>
-  </si>
-  <si>
-    <t>distance: 6.670865, power: 27.39529, speed pen: -0.02646348, set bonus: 0.05, spikeTime: 0.2379046, speed: 28.04m/s / 62.72mph</t>
-  </si>
-  <si>
-    <t>distance: 6.613571, power: 28.5898, speed pen: -0.02730619, set bonus: 0.05, spikeTime: 0.226193, speed: 29.24m/s / 65.41mph</t>
-  </si>
-  <si>
-    <t>distance: 6.654432, power: 27.83541, speed pen: -0.01952879, set bonus: 0.05, spikeTime: 0.2319944, speed: 28.68m/s / 64.16mph</t>
-  </si>
-  <si>
-    <t>distance: 6.674328, power: 28.60008, speed pen: -0.01299713, set bonus: 0.05, spikeTime: 0.2250403, speed: 29.66m/s / 66.34mph</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Player Skill</t>
   </si>
@@ -122,12 +74,63 @@
   </si>
   <si>
     <t>athletePower</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>randVar</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>speed pen</t>
+  </si>
+  <si>
+    <t>set bonus</t>
+  </si>
+  <si>
+    <t>spikeTime</t>
+  </si>
+  <si>
+    <t>speed (m/s)</t>
+  </si>
+  <si>
+    <t>speed (mph)</t>
+  </si>
+  <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>maxVar</t>
+  </si>
+  <si>
+    <t>adjPow</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>adjSet</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>skill2val</t>
+  </si>
+  <si>
+    <t>check4dec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,13 +160,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -180,6 +191,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -502,7 +530,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -518,40 +546,40 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -594,16 +622,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -625,90 +653,489 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19289AF4-DE8A-4F06-880E-3024ABD8F25C}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="8.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>9.3537289999999995</v>
+      </c>
+      <c r="B2">
+        <v>-0.38289210000000001</v>
+      </c>
+      <c r="C2">
+        <v>27.61711</v>
+      </c>
+      <c r="D2">
+        <v>-1.670311E-2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.34444659999999999</v>
+      </c>
+      <c r="G2">
+        <v>27.16</v>
+      </c>
+      <c r="H2">
+        <v>60.75</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>7</v>
+      </c>
+      <c r="M2">
+        <f>2+(0.1-2)*(K2/10)</f>
+        <v>0.67000000000000015</v>
+      </c>
+      <c r="N2">
+        <f>MIN(MAX(L2+B2,1),10)</f>
+        <v>6.6171078999999997</v>
+      </c>
+      <c r="O2">
+        <f>IF(J2,0.05,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f>(N2-'Skill to Value'!C$3)*('Skill to Value'!F$3-'Skill to Value'!E$3)/('Skill to Value'!D$3-'Skill to Value'!C$3)+'Skill to Value'!E$3</f>
+        <v>27.617107900000001</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>A2/(P2*(1-(ABS(D2)-O2)))</f>
+        <v>0.34444661481034827</v>
+      </c>
+      <c r="R2" t="b">
+        <f>ROUND(F2,4)=ROUND(Q2,4)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>15</v>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>9.9894079999999992</v>
+      </c>
+      <c r="B3">
+        <v>-3.7250100000000001E-2</v>
+      </c>
+      <c r="C3">
+        <v>27.96275</v>
+      </c>
+      <c r="D3">
+        <v>-1.9782629999999999E-2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.36444959999999998</v>
+      </c>
+      <c r="G3">
+        <v>27.41</v>
+      </c>
+      <c r="H3">
+        <v>61.31</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M8" si="0">2+(0.1-2)*(K3/10)</f>
+        <v>0.67000000000000015</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N8" si="1">MIN(MAX(L3+B3,1),10)</f>
+        <v>6.9627499000000004</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O8" si="2">IF(J3,0.05,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>(N3-'Skill to Value'!C$3)*('Skill to Value'!F$3-'Skill to Value'!E$3)/('Skill to Value'!D$3-'Skill to Value'!C$3)+'Skill to Value'!E$3</f>
+        <v>27.962749899999999</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" ref="Q3:Q8" si="3">A3/(P3*(1-(ABS(D3)-O3)))</f>
+        <v>0.36444960087067324</v>
+      </c>
+      <c r="R3" t="b">
+        <f t="shared" ref="R3:R8" si="4">ROUND(F3,4)=ROUND(Q3,4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>6.6992789999999998</v>
+      </c>
+      <c r="B4">
+        <v>-6.1465319999999997E-2</v>
+      </c>
+      <c r="C4">
+        <v>27.93853</v>
+      </c>
+      <c r="D4">
+        <v>-1.526279E-2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.24350289999999999</v>
+      </c>
+      <c r="G4">
+        <v>27.51</v>
+      </c>
+      <c r="H4">
+        <v>61.54</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <v>7</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0.67000000000000015</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>6.9385346800000001</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f>(N4-'Skill to Value'!C$3)*('Skill to Value'!F$3-'Skill to Value'!E$3)/('Skill to Value'!D$3-'Skill to Value'!C$3)+'Skill to Value'!E$3</f>
+        <v>27.93853468</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="3"/>
+        <v>0.2435028740950228</v>
+      </c>
+      <c r="R4" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>10.0289</v>
+      </c>
+      <c r="B5">
+        <v>0.31448999999999999</v>
+      </c>
+      <c r="C5">
+        <v>28.314489999999999</v>
+      </c>
+      <c r="D5">
+        <v>-1.317898E-2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.3589271</v>
+      </c>
+      <c r="G5">
+        <v>27.94</v>
+      </c>
+      <c r="H5">
+        <v>62.5</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0.67000000000000015</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>7.3144900000000002</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f>(N5-'Skill to Value'!C$3)*('Skill to Value'!F$3-'Skill to Value'!E$3)/('Skill to Value'!D$3-'Skill to Value'!C$3)+'Skill to Value'!E$3</f>
+        <v>28.314489999999999</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.35892703029020528</v>
+      </c>
+      <c r="R5" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>6.4994930000000002</v>
+      </c>
+      <c r="B6">
+        <v>0.17522389999999999</v>
+      </c>
+      <c r="C6">
+        <v>28.175219999999999</v>
+      </c>
+      <c r="D6">
+        <v>-2.258897E-2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.23601240000000001</v>
+      </c>
+      <c r="G6">
+        <v>27.54</v>
+      </c>
+      <c r="H6">
+        <v>61.6</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <v>7</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.67000000000000015</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>7.1752238999999998</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f>(N6-'Skill to Value'!C$3)*('Skill to Value'!F$3-'Skill to Value'!E$3)/('Skill to Value'!D$3-'Skill to Value'!C$3)+'Skill to Value'!E$3</f>
+        <v>28.175223899999999</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.23601242580456191</v>
+      </c>
+      <c r="R6" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>6.4744270000000004</v>
+      </c>
+      <c r="B7">
+        <v>-0.19184329999999999</v>
+      </c>
+      <c r="C7">
+        <v>27.808160000000001</v>
+      </c>
+      <c r="D7">
+        <v>-2.693108E-2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.2392685</v>
+      </c>
+      <c r="G7">
+        <v>27.06</v>
+      </c>
+      <c r="H7">
+        <v>60.53</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0.67000000000000015</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>6.8081566999999996</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f>(N7-'Skill to Value'!C$3)*('Skill to Value'!F$3-'Skill to Value'!E$3)/('Skill to Value'!D$3-'Skill to Value'!C$3)+'Skill to Value'!E$3</f>
+        <v>27.808156699999998</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.23926850450243278</v>
+      </c>
+      <c r="R7" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>6.6844460000000003</v>
+      </c>
+      <c r="B8">
+        <v>-0.137458</v>
+      </c>
+      <c r="C8">
+        <v>27.862539999999999</v>
+      </c>
+      <c r="D8">
+        <v>-1.5332200000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.24364359999999999</v>
+      </c>
+      <c r="G8">
+        <v>27.44</v>
+      </c>
+      <c r="H8">
+        <v>61.37</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.67000000000000015</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>6.8625420000000004</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f>(N8-'Skill to Value'!C$3)*('Skill to Value'!F$3-'Skill to Value'!E$3)/('Skill to Value'!D$3-'Skill to Value'!C$3)+'Skill to Value'!E$3</f>
+        <v>27.862542000000001</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.24364356581847257</v>
+      </c>
+      <c r="R8" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More attempted work on formula
</commit_message>
<xml_diff>
--- a/Resources/Spike Speed Tracker.xlsx
+++ b/Resources/Spike Speed Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89169FD0-A655-44B2-913B-99C77866917F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F5872F-1B39-4604-899D-E3C078F15A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>Player Skill</t>
   </si>
@@ -222,14 +222,18 @@
   </si>
   <si>
     <t>SToV</t>
+  </si>
+  <si>
+    <t>SToV(p_adj,rng_sp)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -260,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -276,6 +280,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -294,6 +300,14 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
@@ -391,26 +405,142 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>239487</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>10887</xdr:rowOff>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>108857</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>27214</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>527957</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>163286</xdr:rowOff>
+          <xdr:col>23</xdr:col>
+          <xdr:colOff>397330</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>179614</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="ScrollBar1" hidden="1">
+            <xdr:cNvPr id="1026" name="timingVar" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
+                  <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC3D9CC4-C673-2085-011A-09056B228883}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>108857</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>27214</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>23</xdr:col>
+          <xdr:colOff>397330</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>179614</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="SpikeSkill" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77EDF033-2FB9-2838-646F-6DC3272F9B1E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>108857</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>27214</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>23</xdr:col>
+          <xdr:colOff>397330</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>179614</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="SpikeTimingWindow" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EDE0BBB-491B-147B-1AFA-49AEB269168D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1404,65 +1534,71 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA744AF-4B66-411A-B034-C8F30C452722}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="20" max="20" width="17.07421875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="T10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1476,8 +1612,11 @@
         <f>D12/100</f>
         <v>0.13</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="T12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1485,23 +1624,40 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>40</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="D14">
+        <v>70</v>
+      </c>
+      <c r="E14" s="6">
+        <f>D14/10</f>
+        <v>7</v>
+      </c>
+      <c r="T14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15" s="6">
+        <f>D15/100</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1509,7 +1665,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1517,7 +1673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1525,7 +1681,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1533,7 +1689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1541,7 +1697,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1549,7 +1705,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1557,7 +1713,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1565,12 +1721,31 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>58</v>
       </c>
       <c r="B24" t="s">
         <v>59</v>
+      </c>
+      <c r="E24" s="5">
+        <f>(E14-'Skill to Value'!C3)*(0-E15)/('Skill to Value'!D3-'Skill to Value'!C3)+E15</f>
+        <v>3.3333333333333326E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="5">
+        <f>(E14-'Skill to Value'!C3)*(0-E15)/('Skill to Value'!D3-'Skill to Value'!C3)+E15</f>
+        <v>3.3333333333333326E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1581,27 +1756,77 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="ScrollBar1">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" linkedCell="D12" r:id="rId5">
+        <control shapeId="1028" r:id="rId4" name="SpikeTimingWindow">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D15" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>239486</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>10886</xdr:rowOff>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>527957</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>163286</xdr:rowOff>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="ScrollBar1"/>
+        <control shapeId="1028" r:id="rId4" name="SpikeTimingWindow"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId6" name="SpikeSkill">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D14" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId6" name="SpikeSkill"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId8" name="timingVar">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId8" name="timingVar"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Spike Speed Penalty by Skill and Timing Variance
Basically, the higher the skill, the less penalty, despite the variance. But the higher the variance, the skill matters for how much impact it will have. This is working as expected. The question becomes: is the penalty base (SpikeTimingWindow) high enough?
</commit_message>
<xml_diff>
--- a/Resources/Spike Speed Tracker.xlsx
+++ b/Resources/Spike Speed Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F5872F-1B39-4604-899D-E3C078F15A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947A92B0-3A0E-480A-88AD-071BD7C6D524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t>Player Skill</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>SToV(p_adj,rng_sp)</t>
+  </si>
+  <si>
+    <t>Timing Variance</t>
+  </si>
+  <si>
+    <t>Skill</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -277,11 +283,11 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -309,6 +315,2032 @@
 
 <file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Spike Speed Penalty</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000"/>
+              <a:t>by</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" baseline="0"/>
+              <a:t> Skill and Timing Variance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$34:$L$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0000000000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.9999999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.9999999999999992E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$35:$L$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.8888888888888889E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7777777777777778E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6666666666666672E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5555555555555556E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4444444444444446E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3333333333333337E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.222222222222222E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.1111111111111111E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8888888888888878E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$36:$L$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7777777777777784E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5555555555555557E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3333333333333338E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1111111111111114E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.888888888888889E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6666666666666669E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.4444444444444441E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.222222222222222E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.9999999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.7777777777777765E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$37:$L$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6666666666666671E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6666666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.6666666666666662E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9999999999999991E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5555555555555566E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1111111111111113E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.666666666666667E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2222222222222227E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.777777777777778E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.888888888888889E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4444444444444446E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5555555555555552E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$39:$L$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4444444444444453E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8888888888888906E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3333333333333338E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7777777777777781E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2222222222222227E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6666666666666672E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1111111111111114E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5555555555555562E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4444444444444446E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$40:$L$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3333333333333327E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.6666666666666654E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9999999999999985E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3333333333333331E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6666666666666663E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9999999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3333333333333327E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6666666666666658E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3333333333333319E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$41:$L$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2222222222222227E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4444444444444453E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6666666666666688E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.8888888888888906E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1111111111111113E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3333333333333336E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5555555555555557E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7777777777777781E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2222222222222223E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$42:$L$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1111111111111113E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2222222222222227E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3333333333333344E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4444444444444453E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5555555555555566E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.666666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.7777777777777784E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8888888888888906E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1111111111111112E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpikeTime!$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpikeTime!$B$43:$L$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-D398-4F6E-A04F-FE773E83B3C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1757280623"/>
+        <c:axId val="1757281103"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1757280623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1757281103"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1757281103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1757280623"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,7 +2444,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>397330</xdr:colOff>
+          <xdr:colOff>397329</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>179614</xdr:rowOff>
         </xdr:to>
@@ -424,7 +2456,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC3D9CC4-C673-2085-011A-09056B228883}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -470,7 +2502,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>397330</xdr:colOff>
+          <xdr:colOff>397329</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>179614</xdr:rowOff>
         </xdr:to>
@@ -482,7 +2514,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77EDF033-2FB9-2838-646F-6DC3272F9B1E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -528,7 +2560,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>397330</xdr:colOff>
+          <xdr:colOff>397329</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>179614</xdr:rowOff>
         </xdr:to>
@@ -540,7 +2572,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EDE0BBB-491B-147B-1AFA-49AEB269168D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -575,6 +2607,42 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>541565</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>16327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1194708</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>168727</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB9B0017-A94F-780F-EFF7-EE054B6C936A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -931,14 +2999,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
@@ -1534,10 +3602,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA744AF-4B66-411A-B034-C8F30C452722}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1606,11 +3674,11 @@
         <v>38</v>
       </c>
       <c r="D12">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="E12">
         <f>D12/100</f>
-        <v>0.13</v>
+        <v>1</v>
       </c>
       <c r="T12" t="s">
         <v>43</v>
@@ -1634,7 +3702,7 @@
       <c r="D14">
         <v>70</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <f>D14/10</f>
         <v>7</v>
       </c>
@@ -1652,7 +3720,7 @@
       <c r="D15">
         <v>10</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <f>D15/100</f>
         <v>0.1</v>
       </c>
@@ -1728,8 +3796,8 @@
       <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="5">
-        <f>(E14-'Skill to Value'!C3)*(0-E15)/('Skill to Value'!D3-'Skill to Value'!C3)+E15</f>
+      <c r="E24" s="4">
+        <f>E12*((E14-'Skill to Value'!C3)*(0-E15)/('Skill to Value'!D3-'Skill to Value'!C3)+E15)</f>
         <v>3.3333333333333326E-2</v>
       </c>
     </row>
@@ -1737,15 +3805,567 @@
       <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <f>(E14-'Skill to Value'!C3)*(0-E15)/('Skill to Value'!D3-'Skill to Value'!C3)+E15</f>
         <v>3.3333333333333326E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0</v>
+      </c>
+      <c r="C33" s="5">
+        <f>B33+0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" ref="D33:L33" si="0">C33+0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="I33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="L33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" s="4">
+        <f>B$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="4">
+        <f>C$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="D34" s="4">
+        <f>D$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="E34" s="4">
+        <f>E$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="F34" s="4">
+        <f>F$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="G34" s="4">
+        <f>G$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0.05</v>
+      </c>
+      <c r="H34" s="4">
+        <f>H$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0.06</v>
+      </c>
+      <c r="I34" s="4">
+        <f>I$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="J34" s="4">
+        <f>J$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0.08</v>
+      </c>
+      <c r="K34" s="4">
+        <f>K$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0.09</v>
+      </c>
+      <c r="L34" s="4">
+        <f>L$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <f>A34+1</f>
+        <v>2</v>
+      </c>
+      <c r="B35" s="4">
+        <f>B$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="4">
+        <f>C$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>8.8888888888888889E-3</v>
+      </c>
+      <c r="D35" s="4">
+        <f>D$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.7777777777777778E-2</v>
+      </c>
+      <c r="E35" s="4">
+        <f>E$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.6666666666666672E-2</v>
+      </c>
+      <c r="F35" s="4">
+        <f>F$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.5555555555555556E-2</v>
+      </c>
+      <c r="G35" s="4">
+        <f>G$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="H35" s="4">
+        <f>H$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="I35" s="4">
+        <f>I$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>6.222222222222222E-2</v>
+      </c>
+      <c r="J35" s="4">
+        <f>J$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>7.1111111111111111E-2</v>
+      </c>
+      <c r="K35" s="4">
+        <f>K$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0.08</v>
+      </c>
+      <c r="L35" s="4">
+        <f>L$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>8.8888888888888878E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <f t="shared" ref="A36:A43" si="1">A35+1</f>
+        <v>3</v>
+      </c>
+      <c r="B36" s="4">
+        <f>B$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="4">
+        <f>C$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>7.7777777777777784E-3</v>
+      </c>
+      <c r="D36" s="4">
+        <f>D$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.5555555555555557E-2</v>
+      </c>
+      <c r="E36" s="4">
+        <f>E$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.3333333333333338E-2</v>
+      </c>
+      <c r="F36" s="4">
+        <f>F$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.1111111111111114E-2</v>
+      </c>
+      <c r="G36" s="4">
+        <f>G$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="H36" s="4">
+        <f>H$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.6666666666666669E-2</v>
+      </c>
+      <c r="I36" s="4">
+        <f>I$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>5.4444444444444441E-2</v>
+      </c>
+      <c r="J36" s="4">
+        <f>J$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>6.222222222222222E-2</v>
+      </c>
+      <c r="K36" s="4">
+        <f>K$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="L36" s="4">
+        <f>L$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>7.7777777777777765E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B37" s="4">
+        <f>B$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="4">
+        <f>C$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="D37" s="4">
+        <f>D$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="E37" s="4">
+        <f>E$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="F37" s="4">
+        <f>F$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.6666666666666668E-2</v>
+      </c>
+      <c r="G37" s="4">
+        <f>G$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H37" s="4">
+        <f>H$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0.04</v>
+      </c>
+      <c r="I37" s="4">
+        <f>I$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.6666666666666662E-2</v>
+      </c>
+      <c r="J37" s="4">
+        <f>J$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>5.333333333333333E-2</v>
+      </c>
+      <c r="K37" s="4">
+        <f>K$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>5.9999999999999991E-2</v>
+      </c>
+      <c r="L37" s="4">
+        <f>L$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B38" s="4">
+        <f>B$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="4">
+        <f>C$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>5.5555555555555566E-3</v>
+      </c>
+      <c r="D38" s="4">
+        <f>D$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.1111111111111113E-2</v>
+      </c>
+      <c r="E38" s="4">
+        <f>E$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.666666666666667E-2</v>
+      </c>
+      <c r="F38" s="4">
+        <f>F$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.2222222222222227E-2</v>
+      </c>
+      <c r="G38" s="4">
+        <f>G$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.777777777777778E-2</v>
+      </c>
+      <c r="H38" s="4">
+        <f>H$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="I38" s="4">
+        <f>I$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="J38" s="4">
+        <f>J$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="K38" s="4">
+        <f>K$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="L38" s="4">
+        <f>L$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B39" s="4">
+        <f>B$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="4">
+        <f>C$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.4444444444444453E-3</v>
+      </c>
+      <c r="D39" s="4">
+        <f>D$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>8.8888888888888906E-3</v>
+      </c>
+      <c r="E39" s="4">
+        <f>E$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.3333333333333338E-2</v>
+      </c>
+      <c r="F39" s="4">
+        <f>F$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.7777777777777781E-2</v>
+      </c>
+      <c r="G39" s="4">
+        <f>G$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.2222222222222227E-2</v>
+      </c>
+      <c r="H39" s="4">
+        <f>H$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.6666666666666672E-2</v>
+      </c>
+      <c r="I39" s="4">
+        <f>I$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.1111111111111114E-2</v>
+      </c>
+      <c r="J39" s="4">
+        <f>J$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.5555555555555562E-2</v>
+      </c>
+      <c r="K39" s="4">
+        <f>K$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0.04</v>
+      </c>
+      <c r="L39" s="4">
+        <f>L$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B40" s="4">
+        <f>B$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C40" s="4">
+        <f>C$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.3333333333333327E-3</v>
+      </c>
+      <c r="D40" s="4">
+        <f>D$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>6.6666666666666654E-3</v>
+      </c>
+      <c r="E40" s="4">
+        <f>E$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>9.9999999999999985E-3</v>
+      </c>
+      <c r="F40" s="4">
+        <f>F$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.3333333333333331E-2</v>
+      </c>
+      <c r="G40" s="4">
+        <f>G$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.6666666666666663E-2</v>
+      </c>
+      <c r="H40" s="4">
+        <f>H$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.9999999999999993E-2</v>
+      </c>
+      <c r="I40" s="4">
+        <f>I$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.3333333333333327E-2</v>
+      </c>
+      <c r="J40" s="4">
+        <f>J$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.6666666666666658E-2</v>
+      </c>
+      <c r="K40" s="4">
+        <f>K$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.9999999999999992E-2</v>
+      </c>
+      <c r="L40" s="4">
+        <f>L$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.3333333333333319E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B41" s="4">
+        <f>B$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C41" s="4">
+        <f>C$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.2222222222222227E-3</v>
+      </c>
+      <c r="D41" s="4">
+        <f>D$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.4444444444444453E-3</v>
+      </c>
+      <c r="E41" s="4">
+        <f>E$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>6.6666666666666688E-3</v>
+      </c>
+      <c r="F41" s="4">
+        <f>F$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>8.8888888888888906E-3</v>
+      </c>
+      <c r="G41" s="4">
+        <f>G$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.1111111111111113E-2</v>
+      </c>
+      <c r="H41" s="4">
+        <f>H$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.3333333333333336E-2</v>
+      </c>
+      <c r="I41" s="4">
+        <f>I$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.5555555555555557E-2</v>
+      </c>
+      <c r="J41" s="4">
+        <f>J$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.7777777777777781E-2</v>
+      </c>
+      <c r="K41" s="4">
+        <f>K$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0.02</v>
+      </c>
+      <c r="L41" s="4">
+        <f>L$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.2222222222222223E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B42" s="4">
+        <f>B$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C42" s="4">
+        <f>C$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.1111111111111113E-3</v>
+      </c>
+      <c r="D42" s="4">
+        <f>D$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>2.2222222222222227E-3</v>
+      </c>
+      <c r="E42" s="4">
+        <f>E$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>3.3333333333333344E-3</v>
+      </c>
+      <c r="F42" s="4">
+        <f>F$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>4.4444444444444453E-3</v>
+      </c>
+      <c r="G42" s="4">
+        <f>G$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>5.5555555555555566E-3</v>
+      </c>
+      <c r="H42" s="4">
+        <f>H$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>6.666666666666668E-3</v>
+      </c>
+      <c r="I42" s="4">
+        <f>I$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>7.7777777777777784E-3</v>
+      </c>
+      <c r="J42" s="4">
+        <f>J$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>8.8888888888888906E-3</v>
+      </c>
+      <c r="K42" s="4">
+        <f>K$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0.01</v>
+      </c>
+      <c r="L42" s="4">
+        <f>L$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>1.1111111111111112E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B43" s="4">
+        <f>B$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
+        <f>C$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <f>D$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="E43" s="4">
+        <f>E$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="F43" s="4">
+        <f>F$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="4">
+        <f>G$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="4">
+        <f>H$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="4">
+        <f>I$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="4">
+        <f>J$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="K43" s="4">
+        <f>K$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
+      </c>
+      <c r="L43" s="4">
+        <f>L$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1756,19 +4376,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId4" name="SpikeTimingWindow">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D15" r:id="rId5">
+        <control shapeId="1026" r:id="rId4" name="timingVar">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
                 <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>13</xdr:row>
+                <xdr:row>9</xdr:row>
                 <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>23</xdr:col>
                 <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>13</xdr:row>
+                <xdr:row>9</xdr:row>
                 <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
@@ -1776,7 +4396,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId4" name="SpikeTimingWindow"/>
+        <control shapeId="1026" r:id="rId4" name="timingVar"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1806,19 +4426,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId8" name="timingVar">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId9">
+        <control shapeId="1028" r:id="rId8" name="SpikeTimingWindow">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D15" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
                 <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:row>13</xdr:row>
                 <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>23</xdr:col>
                 <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:row>13</xdr:row>
                 <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
@@ -1826,7 +4446,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId8" name="timingVar"/>
+        <control shapeId="1028" r:id="rId8" name="SpikeTimingWindow"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Playing around with curves and calculations
Also added logging for other debug elements not currently captured.
Made some notes in the Excel about potential calculation adjustments
Ultimately:  what should the curves look like???
that is, at the best skill, what should the penalty be?
</commit_message>
<xml_diff>
--- a/Resources/Spike Speed Tracker.xlsx
+++ b/Resources/Spike Speed Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947A92B0-3A0E-480A-88AD-071BD7C6D524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C382AE5-64B6-4192-BBBC-BE7D864BFBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>Player Skill</t>
   </si>
@@ -231,17 +231,39 @@
   </si>
   <si>
     <t>Skill</t>
+  </si>
+  <si>
+    <t>Revisions</t>
+  </si>
+  <si>
+    <t>Don't need to subtract one, the animation only can run once</t>
+  </si>
+  <si>
+    <t>Spike Speed (mph)</t>
+  </si>
+  <si>
+    <t>Spike Speed (m/s)</t>
+  </si>
+  <si>
+    <t>Consider changing window from 0.1 to 0.25 for more variance and therefore effect on mis-timing</t>
+  </si>
+  <si>
+    <t>Range is -0.4 to -0.8, which means 20% - 60% of animation curve</t>
+  </si>
+  <si>
+    <t>REAL QUESTION:  what should the curve actually look like???</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,16 +271,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -266,11 +310,142 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,12 +463,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -306,7 +551,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -314,6 +559,18 @@
 </file>
 
 <file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
@@ -484,34 +741,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0000000000000002E-2</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0000000000000004E-2</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0000000000000006E-2</c:v>
+                  <c:v>7.5000000000000011E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0000000000000008E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.05</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.06</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.9999999999999993E-2</c:v>
+                  <c:v>0.17499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.08</c:v>
+                  <c:v>0.19999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.09</c:v>
+                  <c:v>0.22499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.9999999999999992E-2</c:v>
+                  <c:v>0.24999999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -519,7 +776,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000000-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -601,34 +858,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.8888888888888889E-3</c:v>
+                  <c:v>2.2222222222222223E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7777777777777778E-2</c:v>
+                  <c:v>4.4444444444444446E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6666666666666672E-2</c:v>
+                  <c:v>6.666666666666668E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5555555555555556E-2</c:v>
+                  <c:v>8.8888888888888892E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4444444444444446E-2</c:v>
+                  <c:v>0.1111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.3333333333333337E-2</c:v>
+                  <c:v>0.13333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.222222222222222E-2</c:v>
+                  <c:v>0.15555555555555553</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.1111111111111111E-2</c:v>
+                  <c:v>0.17777777777777776</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.08</c:v>
+                  <c:v>0.19999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.8888888888888878E-2</c:v>
+                  <c:v>0.22222222222222218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -636,7 +893,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000001-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -718,34 +975,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.7777777777777784E-3</c:v>
+                  <c:v>1.9444444444444445E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5555555555555557E-2</c:v>
+                  <c:v>3.888888888888889E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3333333333333338E-2</c:v>
+                  <c:v>5.8333333333333341E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1111111111111114E-2</c:v>
+                  <c:v>7.7777777777777779E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.888888888888889E-2</c:v>
+                  <c:v>9.7222222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6666666666666669E-2</c:v>
+                  <c:v>0.11666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4444444444444441E-2</c:v>
+                  <c:v>0.1361111111111111</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.222222222222222E-2</c:v>
+                  <c:v>0.15555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9999999999999993E-2</c:v>
+                  <c:v>0.17499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.7777777777777765E-2</c:v>
+                  <c:v>0.19444444444444442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -753,7 +1010,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000002-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -835,34 +1092,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.6666666666666671E-3</c:v>
+                  <c:v>1.666666666666667E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3333333333333334E-2</c:v>
+                  <c:v>3.333333333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0000000000000004E-2</c:v>
+                  <c:v>5.000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6666666666666668E-2</c:v>
+                  <c:v>6.666666666666668E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3333333333333333E-2</c:v>
+                  <c:v>8.3333333333333343E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.04</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.6666666666666662E-2</c:v>
+                  <c:v>0.11666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.333333333333333E-2</c:v>
+                  <c:v>0.13333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.9999999999999991E-2</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.6666666666666652E-2</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -870,7 +1127,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000003-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -952,34 +1209,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5555555555555566E-3</c:v>
+                  <c:v>1.388888888888889E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1111111111111113E-2</c:v>
+                  <c:v>2.777777777777778E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.666666666666667E-2</c:v>
+                  <c:v>4.1666666666666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2222222222222227E-2</c:v>
+                  <c:v>5.5555555555555559E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.777777777777778E-2</c:v>
+                  <c:v>6.9444444444444448E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3333333333333333E-2</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.888888888888889E-2</c:v>
+                  <c:v>9.7222222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4444444444444446E-2</c:v>
+                  <c:v>0.1111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9999999999999996E-2</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>0.13888888888888887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -987,7 +1244,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000004-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1069,34 +1326,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4444444444444453E-3</c:v>
+                  <c:v>1.1111111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.8888888888888906E-3</c:v>
+                  <c:v>2.2222222222222223E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3333333333333338E-2</c:v>
+                  <c:v>3.333333333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7777777777777781E-2</c:v>
+                  <c:v>4.4444444444444446E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2222222222222227E-2</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.6666666666666672E-2</c:v>
+                  <c:v>6.6666666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1111111111111114E-2</c:v>
+                  <c:v>7.7777777777777765E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5555555555555562E-2</c:v>
+                  <c:v>8.8888888888888878E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.04</c:v>
+                  <c:v>9.9999999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4444444444444446E-2</c:v>
+                  <c:v>0.11111111111111109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1104,7 +1361,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000005-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1188,34 +1445,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3333333333333327E-3</c:v>
+                  <c:v>8.333333333333335E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.6666666666666654E-3</c:v>
+                  <c:v>1.666666666666667E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9999999999999985E-3</c:v>
+                  <c:v>2.5000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3333333333333331E-2</c:v>
+                  <c:v>3.333333333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6666666666666663E-2</c:v>
+                  <c:v>4.1666666666666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9999999999999993E-2</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3333333333333327E-2</c:v>
+                  <c:v>5.8333333333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.6666666666666658E-2</c:v>
+                  <c:v>6.6666666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.9999999999999992E-2</c:v>
+                  <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.3333333333333319E-2</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1223,7 +1480,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000006-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1307,34 +1564,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2222222222222227E-3</c:v>
+                  <c:v>5.5555555555555558E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4444444444444453E-3</c:v>
+                  <c:v>1.1111111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6666666666666688E-3</c:v>
+                  <c:v>1.666666666666667E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.8888888888888906E-3</c:v>
+                  <c:v>2.2222222222222223E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1111111111111113E-2</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3333333333333336E-2</c:v>
+                  <c:v>3.3333333333333333E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5555555555555557E-2</c:v>
+                  <c:v>3.8888888888888883E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7777777777777781E-2</c:v>
+                  <c:v>4.4444444444444439E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.02</c:v>
+                  <c:v>4.9999999999999989E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2222222222222223E-2</c:v>
+                  <c:v>5.5555555555555546E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1342,7 +1599,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000007-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1426,34 +1683,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1111111111111113E-3</c:v>
+                  <c:v>2.7777777777777792E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2222222222222227E-3</c:v>
+                  <c:v>5.5555555555555584E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3333333333333344E-3</c:v>
+                  <c:v>8.3333333333333384E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4444444444444453E-3</c:v>
+                  <c:v>1.1111111111111117E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5555555555555566E-3</c:v>
+                  <c:v>1.3888888888888895E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.666666666666668E-3</c:v>
+                  <c:v>1.6666666666666673E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.7777777777777784E-3</c:v>
+                  <c:v>1.9444444444444452E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.8888888888888906E-3</c:v>
+                  <c:v>2.222222222222223E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.01</c:v>
+                  <c:v>2.5000000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1111111111111112E-2</c:v>
+                  <c:v>2.7777777777777787E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1461,7 +1718,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000008-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1580,7 +1837,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-D398-4F6E-A04F-FE773E83B3C8}"/>
+              <c16:uniqueId val="{00000009-4489-4FE2-AFC1-550A056DB691}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1651,7 +1908,6 @@
         <c:axId val="1757281103"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2398,7 +2654,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>531118</xdr:colOff>
+      <xdr:colOff>531117</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>73567</xdr:rowOff>
     </xdr:to>
@@ -2610,26 +2866,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>541565</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>16327</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1194708</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>168727</xdr:rowOff>
+      <xdr:colOff>653143</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB9B0017-A94F-780F-EFF7-EE054B6C936A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73B328F1-1E4F-4931-B1AC-E69E81D87BED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2643,6 +2901,180 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>108857</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>27214</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>23</xdr:col>
+          <xdr:colOff>397329</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>179614</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="athletePower" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25D22484-A5B9-9D3C-E19C-489B87EB85DA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>108857</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>27214</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>23</xdr:col>
+          <xdr:colOff>397329</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>179614</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="distance" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D67F0B95-100D-2902-5D2C-D8F04A18B5B6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>20</xdr:col>
+          <xdr:colOff>119743</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>152399</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>22</xdr:col>
+          <xdr:colOff>185057</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>59871</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="setPassAdjustment" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -3109,11 +3541,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19289AF4-DE8A-4F06-880E-3024ABD8F25C}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3291,7 +3723,7 @@
         <v>27.962749899999999</v>
       </c>
       <c r="Q3" s="2">
-        <f t="shared" ref="Q3:Q8" si="3">A3/(P3*(1-(ABS(D3)-O3)))</f>
+        <f t="shared" ref="Q3:Q9" si="3">A3/(P3*(1-(ABS(D3)-O3)))</f>
         <v>0.36444960087067324</v>
       </c>
       <c r="R3" t="b">
@@ -3592,6 +4024,12 @@
       <c r="R8" t="b">
         <f t="shared" si="4"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="Q9" s="2">
+        <f ca="1">SpikeTime!E22/(SpikeTime!E26*(1-(ABS(SpikeTime!E24)-SpikeTime!E20)))</f>
+        <v>0.21567217828900073</v>
       </c>
     </row>
   </sheetData>
@@ -3602,14 +4040,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA744AF-4B66-411A-B034-C8F30C452722}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="5" max="5" width="9.15234375" customWidth="1"/>
     <col min="20" max="20" width="17.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3720,9 +4159,8 @@
       <c r="D15">
         <v>10</v>
       </c>
-      <c r="E15" s="5">
-        <f>D15/100</f>
-        <v>0.1</v>
+      <c r="E15" s="4">
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.4">
@@ -3732,64 +4170,109 @@
       <c r="B16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="T16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>46</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E17">
+        <f>2+(0.1-2)*(E14/10)</f>
+        <v>0.67000000000000015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E18" s="4">
+        <f ca="1">RANDBETWEEN(-E17*100,E17*100)/100</f>
+        <v>-0.18</v>
+      </c>
+      <c r="T18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>49</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E19" s="5">
+        <f ca="1">MIN(MAX(E27+E18,1),10)</f>
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>51</v>
       </c>
       <c r="B20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>IF(D20,0.05,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>53</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E21" s="2">
+        <f ca="1">E22/(E26*(1-E24-E20))</f>
+        <v>0.21567217828900073</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>54</v>
       </c>
       <c r="B22" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="D22">
+        <v>55</v>
+      </c>
+      <c r="E22" s="5">
+        <f>D22/10</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>56</v>
       </c>
       <c r="B23" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -3798,577 +4281,643 @@
       </c>
       <c r="E24" s="4">
         <f>E12*((E14-'Skill to Value'!C3)*(0-E15)/('Skill to Value'!D3-'Skill to Value'!C3)+E15)</f>
-        <v>3.3333333333333326E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+        <v>8.3333333333333343E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="4">
-        <f>(E14-'Skill to Value'!C3)*(0-E15)/('Skill to Value'!D3-'Skill to Value'!C3)+E15</f>
-        <v>3.3333333333333326E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+        <f ca="1">(E19-'Skill to Value'!C3)*(E23-D23)/('Skill to Value'!D3-'Skill to Value'!C3)+D23</f>
+        <v>27.82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>70</v>
+      </c>
+      <c r="E27" s="5">
+        <f>D27/10</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="26">
+        <f ca="1">E22/E21</f>
+        <v>25.501666666666665</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="26">
+        <f ca="1">E28*2.23694</f>
+        <v>57.045698233333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+    <row r="33" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="8">
         <v>0</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="8">
         <f>B33+0.1</f>
         <v>0.1</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="14">
         <f t="shared" ref="D33:L33" si="0">C33+0.1</f>
         <v>0.2</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="15">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="15">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="15">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H33" s="15">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I33" s="15">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="J33" s="5">
+      <c r="J33" s="16">
         <f t="shared" si="0"/>
         <v>0.79999999999999993</v>
       </c>
-      <c r="K33" s="5">
+      <c r="K33" s="8">
         <f t="shared" si="0"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="L33" s="5">
+      <c r="L33" s="8">
         <f t="shared" si="0"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A34">
+    <row r="34" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="7">
         <v>1</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="11">
         <f>B$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="9">
         <f>C$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.0000000000000002E-2</v>
-      </c>
-      <c r="D34" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D34" s="17">
         <f>D$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="E34" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="E34" s="18">
         <f>E$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.0000000000000006E-2</v>
-      </c>
-      <c r="F34" s="4">
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="F34" s="18">
         <f>F$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.0000000000000008E-2</v>
-      </c>
-      <c r="G34" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G34" s="18">
         <f>G$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.05</v>
-      </c>
-      <c r="H34" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="H34" s="18">
         <f>H$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.06</v>
-      </c>
-      <c r="I34" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="I34" s="18">
         <f>I$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.9999999999999993E-2</v>
-      </c>
-      <c r="J34" s="4">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="J34" s="19">
         <f>J$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.08</v>
-      </c>
-      <c r="K34" s="4">
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="K34" s="9">
         <f>K$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.09</v>
-      </c>
-      <c r="L34" s="4">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="L34" s="9">
         <f>L$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>9.9999999999999992E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A35">
+        <v>0.24999999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="7">
         <f>A34+1</f>
         <v>2</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="12">
         <f>B$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="10">
         <f>C$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.8888888888888889E-3</v>
-      </c>
-      <c r="D35" s="4">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="D35" s="20">
         <f>D$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.7777777777777778E-2</v>
-      </c>
-      <c r="E35" s="4">
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="E35" s="21">
         <f>E$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.6666666666666672E-2</v>
-      </c>
-      <c r="F35" s="4">
+        <v>6.666666666666668E-2</v>
+      </c>
+      <c r="F35" s="21">
         <f>F$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.5555555555555556E-2</v>
-      </c>
-      <c r="G35" s="4">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="G35" s="21">
         <f>G$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.4444444444444446E-2</v>
-      </c>
-      <c r="H35" s="4">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="H35" s="21">
         <f>H$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.3333333333333337E-2</v>
-      </c>
-      <c r="I35" s="4">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="I35" s="21">
         <f>I$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.222222222222222E-2</v>
-      </c>
-      <c r="J35" s="4">
+        <v>0.15555555555555553</v>
+      </c>
+      <c r="J35" s="22">
         <f>J$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>7.1111111111111111E-2</v>
-      </c>
-      <c r="K35" s="4">
+        <v>0.17777777777777776</v>
+      </c>
+      <c r="K35" s="10">
         <f>K$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.08</v>
-      </c>
-      <c r="L35" s="4">
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="L35" s="10">
         <f>L$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.8888888888888878E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A36">
+        <v>0.22222222222222218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="7">
         <f t="shared" ref="A36:A43" si="1">A35+1</f>
         <v>3</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="12">
         <f>B$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="10">
         <f>C$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>7.7777777777777784E-3</v>
-      </c>
-      <c r="D36" s="4">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="D36" s="20">
         <f>D$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.5555555555555557E-2</v>
-      </c>
-      <c r="E36" s="4">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="E36" s="21">
         <f>E$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.3333333333333338E-2</v>
-      </c>
-      <c r="F36" s="4">
+        <v>5.8333333333333341E-2</v>
+      </c>
+      <c r="F36" s="21">
         <f>F$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.1111111111111114E-2</v>
-      </c>
-      <c r="G36" s="4">
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="G36" s="21">
         <f>G$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.888888888888889E-2</v>
-      </c>
-      <c r="H36" s="4">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="H36" s="21">
         <f>H$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.6666666666666669E-2</v>
-      </c>
-      <c r="I36" s="4">
+        <v>0.11666666666666667</v>
+      </c>
+      <c r="I36" s="21">
         <f>I$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.4444444444444441E-2</v>
-      </c>
-      <c r="J36" s="4">
+        <v>0.1361111111111111</v>
+      </c>
+      <c r="J36" s="22">
         <f>J$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.222222222222222E-2</v>
-      </c>
-      <c r="K36" s="4">
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="K36" s="10">
         <f>K$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.9999999999999993E-2</v>
-      </c>
-      <c r="L36" s="4">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="L36" s="10">
         <f>L$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>7.7777777777777765E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A37">
+        <v>0.19444444444444442</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="12">
         <f>B$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="10">
         <f>C$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.6666666666666671E-3</v>
-      </c>
-      <c r="D37" s="4">
+        <v>1.666666666666667E-2</v>
+      </c>
+      <c r="D37" s="20">
         <f>D$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.3333333333333334E-2</v>
-      </c>
-      <c r="E37" s="4">
+        <v>3.333333333333334E-2</v>
+      </c>
+      <c r="E37" s="21">
         <f>E$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="F37" s="4">
+        <v>5.000000000000001E-2</v>
+      </c>
+      <c r="F37" s="21">
         <f>F$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.6666666666666668E-2</v>
-      </c>
-      <c r="G37" s="4">
+        <v>6.666666666666668E-2</v>
+      </c>
+      <c r="G37" s="21">
         <f>G$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="H37" s="4">
+        <v>8.3333333333333343E-2</v>
+      </c>
+      <c r="H37" s="21">
         <f>H$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.04</v>
-      </c>
-      <c r="I37" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I37" s="21">
         <f>I$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.6666666666666662E-2</v>
-      </c>
-      <c r="J37" s="4">
+        <v>0.11666666666666667</v>
+      </c>
+      <c r="J37" s="22">
         <f>J$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.333333333333333E-2</v>
-      </c>
-      <c r="K37" s="4">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="K37" s="10">
         <f>K$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.9999999999999991E-2</v>
-      </c>
-      <c r="L37" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L37" s="10">
         <f>L$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.6666666666666652E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A38">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="12">
         <f>B$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="10">
         <f>C$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.5555555555555566E-3</v>
-      </c>
-      <c r="D38" s="4">
+        <v>1.388888888888889E-2</v>
+      </c>
+      <c r="D38" s="20">
         <f>D$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.1111111111111113E-2</v>
-      </c>
-      <c r="E38" s="4">
+        <v>2.777777777777778E-2</v>
+      </c>
+      <c r="E38" s="21">
         <f>E$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.666666666666667E-2</v>
-      </c>
-      <c r="F38" s="4">
+        <v>4.1666666666666671E-2</v>
+      </c>
+      <c r="F38" s="21">
         <f>F$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.2222222222222227E-2</v>
-      </c>
-      <c r="G38" s="4">
+        <v>5.5555555555555559E-2</v>
+      </c>
+      <c r="G38" s="21">
         <f>G$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.777777777777778E-2</v>
-      </c>
-      <c r="H38" s="4">
+        <v>6.9444444444444448E-2</v>
+      </c>
+      <c r="H38" s="21">
         <f>H$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="I38" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I38" s="21">
         <f>I$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.888888888888889E-2</v>
-      </c>
-      <c r="J38" s="4">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="J38" s="22">
         <f>J$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.4444444444444446E-2</v>
-      </c>
-      <c r="K38" s="4">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K38" s="10">
         <f>K$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.9999999999999996E-2</v>
-      </c>
-      <c r="L38" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="L38" s="10">
         <f>L$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.5555555555555552E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A39">
+        <v>0.13888888888888887</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="12">
         <f>B$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="10">
         <f>C$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.4444444444444453E-3</v>
-      </c>
-      <c r="D39" s="4">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="D39" s="20">
         <f>D$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.8888888888888906E-3</v>
-      </c>
-      <c r="E39" s="4">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="E39" s="21">
         <f>E$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.3333333333333338E-2</v>
-      </c>
-      <c r="F39" s="4">
+        <v>3.333333333333334E-2</v>
+      </c>
+      <c r="F39" s="21">
         <f>F$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.7777777777777781E-2</v>
-      </c>
-      <c r="G39" s="4">
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="G39" s="21">
         <f>G$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.2222222222222227E-2</v>
-      </c>
-      <c r="H39" s="4">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="H39" s="21">
         <f>H$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.6666666666666672E-2</v>
-      </c>
-      <c r="I39" s="4">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I39" s="21">
         <f>I$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.1111111111111114E-2</v>
-      </c>
-      <c r="J39" s="4">
+        <v>7.7777777777777765E-2</v>
+      </c>
+      <c r="J39" s="22">
         <f>J$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.5555555555555562E-2</v>
-      </c>
-      <c r="K39" s="4">
+        <v>8.8888888888888878E-2</v>
+      </c>
+      <c r="K39" s="10">
         <f>K$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.04</v>
-      </c>
-      <c r="L39" s="4">
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="L39" s="10">
         <f>L$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.4444444444444446E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A40">
+        <v>0.11111111111111109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="7">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="12">
         <f>B$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="10">
         <f>C$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.3333333333333327E-3</v>
-      </c>
-      <c r="D40" s="4">
+        <v>8.333333333333335E-3</v>
+      </c>
+      <c r="D40" s="20">
         <f>D$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.6666666666666654E-3</v>
-      </c>
-      <c r="E40" s="4">
+        <v>1.666666666666667E-2</v>
+      </c>
+      <c r="E40" s="21">
         <f>E$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>9.9999999999999985E-3</v>
-      </c>
-      <c r="F40" s="4">
+        <v>2.5000000000000005E-2</v>
+      </c>
+      <c r="F40" s="21">
         <f>F$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.3333333333333331E-2</v>
-      </c>
-      <c r="G40" s="4">
+        <v>3.333333333333334E-2</v>
+      </c>
+      <c r="G40" s="21">
         <f>G$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.6666666666666663E-2</v>
-      </c>
-      <c r="H40" s="4">
+        <v>4.1666666666666671E-2</v>
+      </c>
+      <c r="H40" s="21">
         <f>H$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.9999999999999993E-2</v>
-      </c>
-      <c r="I40" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="I40" s="21">
         <f>I$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.3333333333333327E-2</v>
-      </c>
-      <c r="J40" s="4">
+        <v>5.8333333333333334E-2</v>
+      </c>
+      <c r="J40" s="22">
         <f>J$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.6666666666666658E-2</v>
-      </c>
-      <c r="K40" s="4">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="K40" s="10">
         <f>K$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.9999999999999992E-2</v>
-      </c>
-      <c r="L40" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L40" s="10">
         <f>L$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.3333333333333319E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A41">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="7">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="12">
         <f>B$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="10">
         <f>C$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.2222222222222227E-3</v>
-      </c>
-      <c r="D41" s="4">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="D41" s="20">
         <f>D$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.4444444444444453E-3</v>
-      </c>
-      <c r="E41" s="4">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="E41" s="21">
         <f>E$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.6666666666666688E-3</v>
-      </c>
-      <c r="F41" s="4">
+        <v>1.666666666666667E-2</v>
+      </c>
+      <c r="F41" s="21">
         <f>F$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.8888888888888906E-3</v>
-      </c>
-      <c r="G41" s="4">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="G41" s="21">
         <f>G$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.1111111111111113E-2</v>
-      </c>
-      <c r="H41" s="4">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H41" s="21">
         <f>H$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.3333333333333336E-2</v>
-      </c>
-      <c r="I41" s="4">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="I41" s="21">
         <f>I$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.5555555555555557E-2</v>
-      </c>
-      <c r="J41" s="4">
+        <v>3.8888888888888883E-2</v>
+      </c>
+      <c r="J41" s="22">
         <f>J$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.7777777777777781E-2</v>
-      </c>
-      <c r="K41" s="4">
+        <v>4.4444444444444439E-2</v>
+      </c>
+      <c r="K41" s="10">
         <f>K$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.02</v>
-      </c>
-      <c r="L41" s="4">
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="L41" s="10">
         <f>L$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.2222222222222223E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A42">
+        <v>5.5555555555555546E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="7">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="12">
         <f>B$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="10">
         <f>C$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.1111111111111113E-3</v>
-      </c>
-      <c r="D42" s="4">
+        <v>2.7777777777777792E-3</v>
+      </c>
+      <c r="D42" s="20">
         <f>D$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.2222222222222227E-3</v>
-      </c>
-      <c r="E42" s="4">
+        <v>5.5555555555555584E-3</v>
+      </c>
+      <c r="E42" s="21">
         <f>E$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.3333333333333344E-3</v>
-      </c>
-      <c r="F42" s="4">
+        <v>8.3333333333333384E-3</v>
+      </c>
+      <c r="F42" s="21">
         <f>F$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.4444444444444453E-3</v>
-      </c>
-      <c r="G42" s="4">
+        <v>1.1111111111111117E-2</v>
+      </c>
+      <c r="G42" s="21">
         <f>G$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.5555555555555566E-3</v>
-      </c>
-      <c r="H42" s="4">
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="H42" s="21">
         <f>H$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.666666666666668E-3</v>
-      </c>
-      <c r="I42" s="4">
+        <v>1.6666666666666673E-2</v>
+      </c>
+      <c r="I42" s="21">
         <f>I$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>7.7777777777777784E-3</v>
-      </c>
-      <c r="J42" s="4">
+        <v>1.9444444444444452E-2</v>
+      </c>
+      <c r="J42" s="22">
         <f>J$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.8888888888888906E-3</v>
-      </c>
-      <c r="K42" s="4">
+        <v>2.222222222222223E-2</v>
+      </c>
+      <c r="K42" s="10">
         <f>K$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.01</v>
-      </c>
-      <c r="L42" s="4">
+        <v>2.5000000000000008E-2</v>
+      </c>
+      <c r="L42" s="10">
         <f>L$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.1111111111111112E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A43">
+        <v>2.7777777777777787E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="7">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="12">
         <f>B$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="10">
         <f>C$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="23">
         <f>D$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="24">
         <f>E$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="24">
         <f>F$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="24">
         <f>G$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="24">
         <f>H$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="24">
         <f>I$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="25">
         <f>J$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="K43" s="4">
+      <c r="K43" s="10">
         <f>K$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="10">
         <f>L$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L44">
+        <f>_xlfn.VAR.P(B34:L43)</f>
+        <v>3.7905092592592604E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A45" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A49" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B34:L43">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND($A34=ROUNDDOWN($E$14,0),B$33=ROUNDDOWN($E$12,1))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -4376,8 +4925,133 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="timingVar">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId5">
+        <control shapeId="1033" r:id="rId4" name="setPassAdjustment">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D20" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>119743</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>22</xdr:col>
+                <xdr:colOff>185057</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>59871</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1033" r:id="rId4" name="setPassAdjustment"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1030" r:id="rId6" name="distance">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D22" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1030" r:id="rId6" name="distance"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1029" r:id="rId8" name="athletePower">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D27" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1029" r:id="rId8" name="athletePower"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId10" name="SpikeTimingWindow">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D15" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId10" name="SpikeTimingWindow"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId12" name="SpikeSkill">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D14" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId12" name="SpikeSkill"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId14" name="timingVar">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
@@ -4396,57 +5070,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="timingVar"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId6" name="SpikeSkill">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D14" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>27214</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>23</xdr:col>
-                <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId6" name="SpikeSkill"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId8" name="SpikeTimingWindow">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D15" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>27214</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>23</xdr:col>
-                <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId8" name="SpikeTimingWindow"/>
+        <control shapeId="1026" r:id="rId14" name="timingVar"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Updates to curves and overall formula - need to implement!
</commit_message>
<xml_diff>
--- a/Resources/Spike Speed Tracker.xlsx
+++ b/Resources/Spike Speed Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881D378C-74AC-4D19-B66E-55B7BCED54DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B978A96-8915-417C-99CF-6C7BF5D60B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>Player Skill</t>
   </si>
@@ -258,16 +258,38 @@
   </si>
   <si>
     <t>Framers</t>
+  </si>
+  <si>
+    <t>Ideal spike point in animation: frame 15</t>
+  </si>
+  <si>
+    <t>So if realistic is just 5 to 19, the variance should be how far off it is to those caps</t>
+  </si>
+  <si>
+    <t>Ideal Spike Point</t>
+  </si>
+  <si>
+    <t>Variance to Ideal</t>
+  </si>
+  <si>
+    <t>Adjustments (penalty, set) Multiplier</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Spike Skill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -288,7 +310,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,13 +324,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF00B0F0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -465,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -537,13 +559,34 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +618,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,10 +635,6 @@
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -692,7 +731,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$34</c:f>
+              <c:f>SpikeTime!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -715,7 +754,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -757,42 +796,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$34:$L$34</c:f>
+              <c:f>SpikeTime!$B$39:$L$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.52500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>0.42499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5000000000000011E-2</c:v>
+                  <c:v>0.32499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1</c:v>
+                  <c:v>0.22499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15</c:v>
+                  <c:v>2.5000000000000022E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17499999999999999</c:v>
+                  <c:v>7.4999999999999956E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.19999999999999998</c:v>
+                  <c:v>0.17499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22499999999999998</c:v>
+                  <c:v>0.27499999999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.24999999999999997</c:v>
+                  <c:v>0.37499999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,7 +848,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$35</c:f>
+              <c:f>SpikeTime!$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -832,7 +871,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -874,42 +913,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$35:$L$35</c:f>
+              <c:f>SpikeTime!$B$40:$L$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.5625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2222222222222223E-2</c:v>
+                  <c:v>0.47250000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4444444444444446E-2</c:v>
+                  <c:v>0.38250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.666666666666668E-2</c:v>
+                  <c:v>0.29249999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.8888888888888892E-2</c:v>
+                  <c:v>0.20249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1111111111111111</c:v>
+                  <c:v>0.1125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13333333333333333</c:v>
+                  <c:v>2.250000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.15555555555555553</c:v>
+                  <c:v>6.7499999999999963E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17777777777777776</c:v>
+                  <c:v>0.15749999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19999999999999996</c:v>
+                  <c:v>0.24749999999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.22222222222222218</c:v>
+                  <c:v>0.33749999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -926,7 +965,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$36</c:f>
+              <c:f>SpikeTime!$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -949,7 +988,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -991,42 +1030,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$36:$L$36</c:f>
+              <c:f>SpikeTime!$B$41:$L$41</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9444444444444445E-2</c:v>
+                  <c:v>0.42000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.888888888888889E-2</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8333333333333341E-2</c:v>
+                  <c:v>0.25999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.7777777777777779E-2</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7222222222222224E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11666666666666667</c:v>
+                  <c:v>2.0000000000000018E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1361111111111111</c:v>
+                  <c:v>5.999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.15555555555555556</c:v>
+                  <c:v>0.13999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.17499999999999999</c:v>
+                  <c:v>0.21999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19444444444444442</c:v>
+                  <c:v>0.29999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1043,7 +1082,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$37</c:f>
+              <c:f>SpikeTime!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1066,7 +1105,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1108,42 +1147,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$37:$L$37</c:f>
+              <c:f>SpikeTime!$B$42:$L$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.4375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.666666666666667E-2</c:v>
+                  <c:v>0.36749999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.333333333333334E-2</c:v>
+                  <c:v>0.29749999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.000000000000001E-2</c:v>
+                  <c:v>0.22749999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.666666666666668E-2</c:v>
+                  <c:v>0.15749999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3333333333333343E-2</c:v>
+                  <c:v>8.7499999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1</c:v>
+                  <c:v>1.7500000000000016E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.11666666666666667</c:v>
+                  <c:v>5.2499999999999963E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13333333333333333</c:v>
+                  <c:v>0.12249999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.15</c:v>
+                  <c:v>0.19249999999999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.2624999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1160,7 +1199,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$38</c:f>
+              <c:f>SpikeTime!$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1183,7 +1222,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1225,42 +1264,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$38:$L$38</c:f>
+              <c:f>SpikeTime!$B$43:$L$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.388888888888889E-2</c:v>
+                  <c:v>0.315</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.777777777777778E-2</c:v>
+                  <c:v>0.255</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1666666666666671E-2</c:v>
+                  <c:v>0.19499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5555555555555559E-2</c:v>
+                  <c:v>0.13499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9444444444444448E-2</c:v>
+                  <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.3333333333333329E-2</c:v>
+                  <c:v>1.5000000000000013E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.7222222222222224E-2</c:v>
+                  <c:v>4.4999999999999971E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1111111111111111</c:v>
+                  <c:v>0.10499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.125</c:v>
+                  <c:v>0.16499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13888888888888887</c:v>
+                  <c:v>0.22499999999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1277,7 +1316,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$39</c:f>
+              <c:f>SpikeTime!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1300,7 +1339,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1342,42 +1381,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$39:$L$39</c:f>
+              <c:f>SpikeTime!$B$44:$L$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1111111111111112E-2</c:v>
+                  <c:v>0.26250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2222222222222223E-2</c:v>
+                  <c:v>0.21249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.333333333333334E-2</c:v>
+                  <c:v>0.16249999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4444444444444446E-2</c:v>
+                  <c:v>0.11249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.6666666666666666E-2</c:v>
+                  <c:v>1.2500000000000011E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.7777777777777765E-2</c:v>
+                  <c:v>3.7499999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.8888888888888878E-2</c:v>
+                  <c:v>8.7499999999999967E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9999999999999978E-2</c:v>
+                  <c:v>0.13749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11111111111111109</c:v>
+                  <c:v>0.18749999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1394,7 +1433,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$40</c:f>
+              <c:f>SpikeTime!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1419,7 +1458,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1461,42 +1500,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$40:$L$40</c:f>
+              <c:f>SpikeTime!$B$45:$L$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.24999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.333333333333335E-3</c:v>
+                  <c:v>0.20999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.666666666666667E-2</c:v>
+                  <c:v>0.16999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5000000000000005E-2</c:v>
+                  <c:v>0.12999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.333333333333334E-2</c:v>
+                  <c:v>8.9999999999999969E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1666666666666671E-2</c:v>
+                  <c:v>4.9999999999999989E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.05</c:v>
+                  <c:v>1.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.8333333333333334E-2</c:v>
+                  <c:v>2.9999999999999975E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.6666666666666666E-2</c:v>
+                  <c:v>6.9999999999999951E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.4999999999999997E-2</c:v>
+                  <c:v>0.10999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.3333333333333329E-2</c:v>
+                  <c:v>0.14999999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1513,7 +1552,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$41</c:f>
+              <c:f>SpikeTime!$A$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1538,7 +1577,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1580,42 +1619,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$41:$L$41</c:f>
+              <c:f>SpikeTime!$B$46:$L$46</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.18750000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5555555555555558E-3</c:v>
+                  <c:v>0.15750000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1111111111111112E-2</c:v>
+                  <c:v>0.1275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.666666666666667E-2</c:v>
+                  <c:v>9.7500000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2222222222222223E-2</c:v>
+                  <c:v>6.7500000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7777777777777776E-2</c:v>
+                  <c:v>3.7500000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3333333333333333E-2</c:v>
+                  <c:v>7.5000000000000075E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8888888888888883E-2</c:v>
+                  <c:v>2.2499999999999989E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4444444444444439E-2</c:v>
+                  <c:v>5.2499999999999991E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9999999999999989E-2</c:v>
+                  <c:v>8.249999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5555555555555546E-2</c:v>
+                  <c:v>0.11249999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1632,7 +1671,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$42</c:f>
+              <c:f>SpikeTime!$A$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1657,7 +1696,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1699,42 +1738,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$42:$L$42</c:f>
+              <c:f>SpikeTime!$B$47:$L$47</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.12499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7777777777777792E-3</c:v>
+                  <c:v>0.10499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.5555555555555584E-3</c:v>
+                  <c:v>8.4999999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.3333333333333384E-3</c:v>
+                  <c:v>6.4999999999999974E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1111111111111117E-2</c:v>
+                  <c:v>4.4999999999999984E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3888888888888895E-2</c:v>
+                  <c:v>2.4999999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6666666666666673E-2</c:v>
+                  <c:v>5.0000000000000036E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9444444444444452E-2</c:v>
+                  <c:v>1.4999999999999987E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.222222222222223E-2</c:v>
+                  <c:v>3.4999999999999976E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5000000000000008E-2</c:v>
+                  <c:v>5.4999999999999973E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.7777777777777787E-2</c:v>
+                  <c:v>7.4999999999999956E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1751,7 +1790,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>SpikeTime!$A$43</c:f>
+              <c:f>SpikeTime!$A$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1776,7 +1815,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SpikeTime!$B$33:$L$33</c:f>
+              <c:f>SpikeTime!$B$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1818,42 +1857,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SpikeTime!$B$43:$L$43</c:f>
+              <c:f>SpikeTime!$B$48:$L$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6.2500000000000056E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.2500000000000047E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4.2500000000000038E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.2500000000000022E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.2500000000000017E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.2500000000000011E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.5000000000000044E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7.5000000000000023E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1.7500000000000009E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2.7500000000000014E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3.7500000000000019E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2829,75 +2868,17 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>20</xdr:col>
-          <xdr:colOff>108857</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>27214</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>23</xdr:col>
-          <xdr:colOff>397329</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>179614</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1028" name="SpikeTimingWindow" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1028"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>653143</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>5443</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2931,13 +2912,13 @@
         <xdr:from>
           <xdr:col>20</xdr:col>
           <xdr:colOff>108857</xdr:colOff>
-          <xdr:row>15</xdr:row>
+          <xdr:row>13</xdr:row>
           <xdr:rowOff>27214</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>23</xdr:col>
           <xdr:colOff>397329</xdr:colOff>
-          <xdr:row>15</xdr:row>
+          <xdr:row>13</xdr:row>
           <xdr:rowOff>179614</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2989,13 +2970,13 @@
         <xdr:from>
           <xdr:col>20</xdr:col>
           <xdr:colOff>108857</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>15</xdr:row>
           <xdr:rowOff>27214</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>23</xdr:col>
           <xdr:colOff>397329</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>15</xdr:row>
           <xdr:rowOff>179614</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -3047,14 +3028,14 @@
         <xdr:from>
           <xdr:col>20</xdr:col>
           <xdr:colOff>119743</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>16</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>22</xdr:col>
           <xdr:colOff>185057</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>59871</xdr:rowOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>59870</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3455,14 +3436,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27" t="s">
+      <c r="D1" s="30"/>
+      <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
@@ -4052,8 +4033,8 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="Q9" s="2">
-        <f ca="1">SpikeTime!E22/(SpikeTime!E25*(1-(ABS(SpikeTime!E24)-SpikeTime!E20)))</f>
-        <v>0.21621621621621623</v>
+        <f ca="1">SpikeTime!E24/(SpikeTime!E26*(1-(ABS(SpikeTime!E27)-SpikeTime!E28)))</f>
+        <v>0.19584300085601195</v>
       </c>
     </row>
   </sheetData>
@@ -4064,10 +4045,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA744AF-4B66-411A-B034-C8F30C452722}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:AE61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4137,838 +4118,1375 @@
         <v>38</v>
       </c>
       <c r="D12">
-        <v>100</v>
-      </c>
-      <c r="E12" s="28">
+        <v>62</v>
+      </c>
+      <c r="E12" s="32">
         <f>D12/100</f>
-        <v>1</v>
+        <v>0.62</v>
       </c>
       <c r="T12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>75</v>
+      </c>
+      <c r="E13">
+        <v>0.625</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14">
-        <v>70</v>
-      </c>
-      <c r="E14" s="5">
-        <f>D14/10</f>
-        <v>7</v>
+        <v>76</v>
+      </c>
+      <c r="E14" s="4">
+        <f>ABS(E12-E13)</f>
+        <v>5.0000000000000044E-3</v>
       </c>
       <c r="T14" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15">
-        <v>10</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0.25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>70</v>
+      </c>
+      <c r="E16" s="5">
+        <f>D16/10</f>
+        <v>7</v>
+      </c>
+      <c r="T16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="E17" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <f>2+(0.1-2)*(E16/10)</f>
+        <v>0.67000000000000015</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="4">
+        <f ca="1">RANDBETWEEN(-E19*100,E19*100)/100</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D21">
+        <v>70</v>
+      </c>
+      <c r="E21" s="5">
+        <f>D21/10</f>
+        <v>7</v>
+      </c>
+      <c r="V21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="5">
+        <f ca="1">MIN(MAX(E21+E20,1),10)</f>
+        <v>7.14</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="V22" s="35">
+        <v>1</v>
+      </c>
+      <c r="W22" s="35">
+        <f>V22+1</f>
+        <v>2</v>
+      </c>
+      <c r="X22" s="35">
+        <f t="shared" ref="X22:AE22" si="0">W22+1</f>
+        <v>3</v>
+      </c>
+      <c r="Y22" s="35">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Z22" s="35">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AA22" s="35">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AB22" s="35">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AC22" s="35">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E17">
-        <f>2+(0.1-2)*(E14/10)</f>
-        <v>0.67000000000000015</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="4">
-        <f ca="1">RANDBETWEEN(-E17*100,E17*100)/100</f>
-        <v>-0.25</v>
-      </c>
-      <c r="T18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="AD22" s="35">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AE22" s="35">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E19" s="5">
-        <f ca="1">MIN(MAX(E26+E18,1),10)</f>
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="29">
-        <f>IF(D20,F20,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="28">
-        <v>0.05</v>
-      </c>
-      <c r="T20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="2">
-        <f ca="1">E22/(E25*(1-(E24-E20)))</f>
-        <v>0.21621621621621623</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
+      <c r="E23" s="2">
+        <f ca="1">E24/(E26*(1-(E27-E28)))</f>
+        <v>0.19584300085601195</v>
+      </c>
+      <c r="U23" s="6">
+        <v>1</v>
+      </c>
+      <c r="V23" s="36">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.89</v>
+      </c>
+      <c r="W23" s="37">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.885000000000002</v>
+      </c>
+      <c r="X23" s="37">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.88</v>
+      </c>
+      <c r="Y23" s="37">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.875</v>
+      </c>
+      <c r="Z23" s="37">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.87</v>
+      </c>
+      <c r="AA23" s="37">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.864999999999998</v>
+      </c>
+      <c r="AB23" s="37">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.86</v>
+      </c>
+      <c r="AC23" s="37">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.855</v>
+      </c>
+      <c r="AD23" s="37">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.85</v>
+      </c>
+      <c r="AE23" s="37">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.844999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>54</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>55</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>55</v>
       </c>
-      <c r="E22" s="5">
-        <f>D22/10</f>
+      <c r="E24" s="5">
+        <f>D24/10</f>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
+      <c r="U24" s="6">
+        <f>U23+1</f>
+        <v>2</v>
+      </c>
+      <c r="V24" s="38">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.901</v>
+      </c>
+      <c r="W24" s="39">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.8965</v>
+      </c>
+      <c r="X24" s="39">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.892000000000003</v>
+      </c>
+      <c r="Y24" s="39">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.887500000000003</v>
+      </c>
+      <c r="Z24" s="39">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.883000000000003</v>
+      </c>
+      <c r="AA24" s="39">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.878500000000003</v>
+      </c>
+      <c r="AB24" s="39">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.874000000000002</v>
+      </c>
+      <c r="AC24" s="39">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.869500000000002</v>
+      </c>
+      <c r="AD24" s="39">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.865000000000002</v>
+      </c>
+      <c r="AE24" s="39">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.860500000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D25" s="26">
         <v>22</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E25" s="26">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="4">
-        <f>E12*((E14-'Skill to Value'!C3)*(0-E15)/('Skill to Value'!D3-'Skill to Value'!C3)+E15)</f>
-        <v>8.3333333333333343E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
+      <c r="U25" s="6">
+        <f t="shared" ref="U25:U32" si="1">U24+1</f>
+        <v>3</v>
+      </c>
+      <c r="V25" s="38">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.911999999999999</v>
+      </c>
+      <c r="W25" s="39">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.908000000000001</v>
+      </c>
+      <c r="X25" s="39">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.904</v>
+      </c>
+      <c r="Y25" s="39">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.9</v>
+      </c>
+      <c r="Z25" s="39">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.896000000000001</v>
+      </c>
+      <c r="AA25" s="39">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.891999999999999</v>
+      </c>
+      <c r="AB25" s="39">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.887999999999998</v>
+      </c>
+      <c r="AC25" s="39">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.884</v>
+      </c>
+      <c r="AD25" s="39">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.88</v>
+      </c>
+      <c r="AE25" s="39">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.876000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="4">
-        <f ca="1">(E19-'Skill to Value'!C3)*(E23-D23)/('Skill to Value'!D3-'Skill to Value'!C3)+D23</f>
-        <v>27.75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26">
-        <v>70</v>
-      </c>
-      <c r="E26" s="5">
-        <f>D26/10</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="25">
-        <f ca="1">E22/E21</f>
-        <v>25.4375</v>
-      </c>
-      <c r="F27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="B28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="25">
-        <f ca="1">E27*2.23694</f>
-        <v>56.902161250000006</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="B32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="7">
-        <v>0</v>
-      </c>
-      <c r="C33" s="7">
-        <f>B33+0.1</f>
-        <v>0.1</v>
-      </c>
-      <c r="D33" s="13">
-        <f t="shared" ref="D33:L33" si="0">C33+0.1</f>
-        <v>0.2</v>
-      </c>
-      <c r="E33" s="14">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="F33" s="14">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="G33" s="14">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="H33" s="14">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="I33" s="14">
-        <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="J33" s="15">
-        <f t="shared" si="0"/>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="K33" s="7">
-        <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="L33" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99999999999999989</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="6">
-        <v>1</v>
-      </c>
-      <c r="B34" s="10">
-        <f>B$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="8">
-        <f>C$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D34" s="16">
-        <f>D$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.05</v>
-      </c>
-      <c r="E34" s="17">
-        <f>E$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>7.5000000000000011E-2</v>
-      </c>
-      <c r="F34" s="17">
-        <f>F$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.1</v>
-      </c>
-      <c r="G34" s="17">
-        <f>G$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.125</v>
-      </c>
-      <c r="H34" s="17">
-        <f>H$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.15</v>
-      </c>
-      <c r="I34" s="17">
-        <f>I$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="J34" s="18">
-        <f>J$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="K34" s="8">
-        <f>K$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="L34" s="8">
-        <f>L$33*(($A34-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.24999999999999997</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="6">
-        <f>A34+1</f>
-        <v>2</v>
-      </c>
-      <c r="B35" s="11">
-        <f>B$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="C35" s="9">
-        <f>C$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.2222222222222223E-2</v>
-      </c>
-      <c r="D35" s="19">
-        <f>D$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.4444444444444446E-2</v>
-      </c>
-      <c r="E35" s="20">
-        <f>E$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.666666666666668E-2</v>
-      </c>
-      <c r="F35" s="20">
-        <f>F$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.8888888888888892E-2</v>
-      </c>
-      <c r="G35" s="20">
-        <f>G$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="H35" s="20">
-        <f>H$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="I35" s="20">
-        <f>I$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.15555555555555553</v>
-      </c>
-      <c r="J35" s="21">
-        <f>J$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.17777777777777776</v>
-      </c>
-      <c r="K35" s="9">
-        <f>K$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="L35" s="9">
-        <f>L$33*(($A35-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.22222222222222218</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="6">
-        <f t="shared" ref="A36:A43" si="1">A35+1</f>
-        <v>3</v>
-      </c>
-      <c r="B36" s="11">
-        <f>B$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="C36" s="9">
-        <f>C$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.9444444444444445E-2</v>
-      </c>
-      <c r="D36" s="19">
-        <f>D$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.888888888888889E-2</v>
-      </c>
-      <c r="E36" s="20">
-        <f>E$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.8333333333333341E-2</v>
-      </c>
-      <c r="F36" s="20">
-        <f>F$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>7.7777777777777779E-2</v>
-      </c>
-      <c r="G36" s="20">
-        <f>G$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="H36" s="20">
-        <f>H$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.11666666666666667</v>
-      </c>
-      <c r="I36" s="20">
-        <f>I$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.1361111111111111</v>
-      </c>
-      <c r="J36" s="21">
-        <f>J$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.15555555555555556</v>
-      </c>
-      <c r="K36" s="9">
-        <f>K$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="L36" s="9">
-        <f>L$33*(($A36-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.19444444444444442</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="6">
+      <c r="E26" s="4">
+        <f ca="1">(E22-'Skill to Value'!C3)*(E25-D25)/('Skill to Value'!D3-'Skill to Value'!C3)+D25</f>
+        <v>28.14</v>
+      </c>
+      <c r="U26" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B37" s="11">
-        <f>B$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="9">
-        <f>C$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.666666666666667E-2</v>
-      </c>
-      <c r="D37" s="19">
-        <f>D$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.333333333333334E-2</v>
-      </c>
-      <c r="E37" s="20">
-        <f>E$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.000000000000001E-2</v>
-      </c>
-      <c r="F37" s="20">
-        <f>F$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.666666666666668E-2</v>
-      </c>
-      <c r="G37" s="20">
-        <f>G$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.3333333333333343E-2</v>
-      </c>
-      <c r="H37" s="20">
-        <f>H$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.1</v>
-      </c>
-      <c r="I37" s="20">
-        <f>I$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.11666666666666667</v>
-      </c>
-      <c r="J37" s="21">
-        <f>J$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="K37" s="9">
-        <f>K$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.15</v>
-      </c>
-      <c r="L37" s="9">
-        <f>L$33*(($A37-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="6">
+      <c r="V26" s="38">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.923000000000002</v>
+      </c>
+      <c r="W26" s="39">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.919500000000003</v>
+      </c>
+      <c r="X26" s="39">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.916</v>
+      </c>
+      <c r="Y26" s="39">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.912500000000001</v>
+      </c>
+      <c r="Z26" s="39">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.909000000000002</v>
+      </c>
+      <c r="AA26" s="39">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.9055</v>
+      </c>
+      <c r="AB26" s="39">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.902000000000001</v>
+      </c>
+      <c r="AC26" s="39">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.898500000000002</v>
+      </c>
+      <c r="AD26" s="39">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.895000000000003</v>
+      </c>
+      <c r="AE26" s="39">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.891500000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="4">
+        <f>E14*((E16-'Skill to Value'!C3)*(D17-E17)/('Skill to Value'!D3-'Skill to Value'!C3)+E17)</f>
+        <v>2.0000000000000013E-3</v>
+      </c>
+      <c r="U27" s="6">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B38" s="11">
-        <f>B$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
+      <c r="V27" s="38">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.934000000000001</v>
+      </c>
+      <c r="W27" s="39">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.931000000000001</v>
+      </c>
+      <c r="X27" s="39">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.928000000000001</v>
+      </c>
+      <c r="Y27" s="39">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.925000000000001</v>
+      </c>
+      <c r="Z27" s="39">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.922000000000001</v>
+      </c>
+      <c r="AA27" s="39">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.919</v>
+      </c>
+      <c r="AB27" s="39">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.916</v>
+      </c>
+      <c r="AC27" s="39">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.913</v>
+      </c>
+      <c r="AD27" s="39">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.91</v>
+      </c>
+      <c r="AE27" s="39">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.907</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="b">
         <v>0</v>
       </c>
-      <c r="C38" s="9">
-        <f>C$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.388888888888889E-2</v>
-      </c>
-      <c r="D38" s="19">
-        <f>D$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.777777777777778E-2</v>
-      </c>
-      <c r="E38" s="20">
-        <f>E$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.1666666666666671E-2</v>
-      </c>
-      <c r="F38" s="20">
-        <f>F$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.5555555555555559E-2</v>
-      </c>
-      <c r="G38" s="20">
-        <f>G$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.9444444444444448E-2</v>
-      </c>
-      <c r="H38" s="20">
-        <f>H$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="I38" s="20">
-        <f>I$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="J38" s="21">
-        <f>J$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="K38" s="9">
-        <f>K$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.125</v>
-      </c>
-      <c r="L38" s="9">
-        <f>L$33*(($A38-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.13888888888888887</v>
+      <c r="E28" s="27">
+        <f>IF(D28,F28,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="U28" s="6">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="V28" s="38">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.945</v>
+      </c>
+      <c r="W28" s="39">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.942500000000003</v>
+      </c>
+      <c r="X28" s="39">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.94</v>
+      </c>
+      <c r="Y28" s="39">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.9375</v>
+      </c>
+      <c r="Z28" s="39">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.935000000000002</v>
+      </c>
+      <c r="AA28" s="39">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.932500000000001</v>
+      </c>
+      <c r="AB28" s="39">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.93</v>
+      </c>
+      <c r="AC28" s="39">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.927500000000002</v>
+      </c>
+      <c r="AD28" s="39">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.925000000000001</v>
+      </c>
+      <c r="AE28" s="39">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.922500000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="4">
+        <f>(1-(E27-E28))</f>
+        <v>0.998</v>
+      </c>
+      <c r="U29" s="6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="V29" s="38">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.956</v>
+      </c>
+      <c r="W29" s="39">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.954000000000001</v>
+      </c>
+      <c r="X29" s="39">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.951999999999998</v>
+      </c>
+      <c r="Y29" s="39">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.95</v>
+      </c>
+      <c r="Z29" s="39">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.948</v>
+      </c>
+      <c r="AA29" s="39">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.946000000000002</v>
+      </c>
+      <c r="AB29" s="39">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.943999999999999</v>
+      </c>
+      <c r="AC29" s="39">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.942</v>
+      </c>
+      <c r="AD29" s="39">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.94</v>
+      </c>
+      <c r="AE29" s="39">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.937999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="25">
+        <f ca="1">E26*E29</f>
+        <v>28.08372</v>
+      </c>
+      <c r="U30" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="V30" s="38">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.966999999999999</v>
+      </c>
+      <c r="W30" s="39">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.965499999999999</v>
+      </c>
+      <c r="X30" s="39">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.963999999999999</v>
+      </c>
+      <c r="Y30" s="39">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.962499999999999</v>
+      </c>
+      <c r="Z30" s="39">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.960999999999999</v>
+      </c>
+      <c r="AA30" s="39">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.959499999999998</v>
+      </c>
+      <c r="AB30" s="39">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.957999999999998</v>
+      </c>
+      <c r="AC30" s="39">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.956499999999998</v>
+      </c>
+      <c r="AD30" s="39">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.954999999999998</v>
+      </c>
+      <c r="AE30" s="39">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.953499999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="U31" s="6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="V31" s="38">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.978000000000002</v>
+      </c>
+      <c r="W31" s="39">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.977</v>
+      </c>
+      <c r="X31" s="39">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.975999999999999</v>
+      </c>
+      <c r="Y31" s="39">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.975000000000001</v>
+      </c>
+      <c r="Z31" s="39">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.974</v>
+      </c>
+      <c r="AA31" s="39">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.972999999999999</v>
+      </c>
+      <c r="AB31" s="39">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.972000000000001</v>
+      </c>
+      <c r="AC31" s="39">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.971</v>
+      </c>
+      <c r="AD31" s="39">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.97</v>
+      </c>
+      <c r="AE31" s="39">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.969000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="25">
+        <f ca="1">E24/E23</f>
+        <v>28.08372</v>
+      </c>
+      <c r="F32" t="s">
+        <v>71</v>
+      </c>
+      <c r="U32" s="6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="V32" s="38">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>21.988999999999997</v>
+      </c>
+      <c r="W32" s="39">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>22.988499999999998</v>
+      </c>
+      <c r="X32" s="39">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>23.988</v>
+      </c>
+      <c r="Y32" s="39">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>24.987499999999997</v>
+      </c>
+      <c r="Z32" s="39">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>25.986999999999998</v>
+      </c>
+      <c r="AA32" s="39">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>26.986499999999999</v>
+      </c>
+      <c r="AB32" s="39">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>27.985999999999997</v>
+      </c>
+      <c r="AC32" s="39">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>28.985499999999998</v>
+      </c>
+      <c r="AD32" s="39">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>29.984999999999999</v>
+      </c>
+      <c r="AE32" s="39">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
+        <v>30.984499999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="25">
+        <f ca="1">E32*2.23694</f>
+        <v>62.821596616800001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0</v>
+      </c>
+      <c r="C38" s="7">
+        <f>B38+0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="D38" s="13">
+        <f t="shared" ref="D38:L38" si="2">C38+0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="E38" s="14">
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F38" s="14">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="G38" s="14">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H38" s="14">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="I38" s="14">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="J38" s="15">
+        <f t="shared" si="2"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="K38" s="7">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="L38" s="7">
+        <f t="shared" si="2"/>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="6">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B39" s="11">
-        <f>B$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="C39" s="9">
-        <f>C$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.1111111111111112E-2</v>
-      </c>
-      <c r="D39" s="19">
-        <f>D$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.2222222222222223E-2</v>
-      </c>
-      <c r="E39" s="20">
-        <f>E$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.333333333333334E-2</v>
-      </c>
-      <c r="F39" s="20">
-        <f>F$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.4444444444444446E-2</v>
-      </c>
-      <c r="G39" s="20">
-        <f>G$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="H39" s="20">
-        <f>H$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="I39" s="20">
-        <f>I$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>7.7777777777777765E-2</v>
-      </c>
-      <c r="J39" s="21">
-        <f>J$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.8888888888888878E-2</v>
-      </c>
-      <c r="K39" s="9">
-        <f>K$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="L39" s="9">
-        <f>L$33*(($A39-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.11111111111111109</v>
+        <v>1</v>
+      </c>
+      <c r="B39" s="10">
+        <f>ABS(B$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.625</v>
+      </c>
+      <c r="C39" s="8">
+        <f>ABS(C$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="D39" s="16">
+        <f>ABS(D$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E39" s="17">
+        <f>ABS(E$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="F39" s="17">
+        <f>ABS(F$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="G39" s="17">
+        <f>ABS(G$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.125</v>
+      </c>
+      <c r="H39" s="17">
+        <f>ABS(H$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="I39" s="17">
+        <f>ABS(I$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>7.4999999999999956E-2</v>
+      </c>
+      <c r="J39" s="18">
+        <f>ABS(J$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.17499999999999993</v>
+      </c>
+      <c r="K39" s="8">
+        <f>ABS(K$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.27499999999999991</v>
+      </c>
+      <c r="L39" s="8">
+        <f>ABS(L$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.37499999999999989</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="6">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>A39+1</f>
+        <v>2</v>
       </c>
       <c r="B40" s="11">
-        <f>B$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
+        <f>ABS(B$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.5625</v>
       </c>
       <c r="C40" s="9">
-        <f>C$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.333333333333335E-3</v>
+        <f>ABS(C$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.47250000000000003</v>
       </c>
       <c r="D40" s="19">
-        <f>D$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.666666666666667E-2</v>
+        <f>ABS(D$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.38250000000000001</v>
       </c>
       <c r="E40" s="20">
-        <f>E$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.5000000000000005E-2</v>
+        <f>ABS(E$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.29249999999999998</v>
       </c>
       <c r="F40" s="20">
-        <f>F$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.333333333333334E-2</v>
+        <f>ABS(F$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.20249999999999999</v>
       </c>
       <c r="G40" s="20">
-        <f>G$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.1666666666666671E-2</v>
+        <f>ABS(G$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.1125</v>
       </c>
       <c r="H40" s="20">
-        <f>H$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0.05</v>
+        <f>ABS(H$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>2.250000000000002E-2</v>
       </c>
       <c r="I40" s="20">
-        <f>I$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.8333333333333334E-2</v>
+        <f>ABS(I$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>6.7499999999999963E-2</v>
       </c>
       <c r="J40" s="21">
-        <f>J$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>6.6666666666666666E-2</v>
+        <f>ABS(J$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.15749999999999995</v>
       </c>
       <c r="K40" s="9">
-        <f>K$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>7.4999999999999997E-2</v>
+        <f>ABS(K$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.24749999999999991</v>
       </c>
       <c r="L40" s="9">
-        <f>L$33*(($A40-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.3333333333333329E-2</v>
+        <f>ABS(L$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.33749999999999991</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" ref="A41:A48" si="3">A40+1</f>
+        <v>3</v>
       </c>
       <c r="B41" s="11">
-        <f>B$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
+        <f>ABS(B$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.5</v>
       </c>
       <c r="C41" s="9">
-        <f>C$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.5555555555555558E-3</v>
+        <f>ABS(C$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.42000000000000004</v>
       </c>
       <c r="D41" s="19">
-        <f>D$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.1111111111111112E-2</v>
+        <f>ABS(D$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.34</v>
       </c>
       <c r="E41" s="20">
-        <f>E$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.666666666666667E-2</v>
+        <f>ABS(E$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.25999999999999995</v>
       </c>
       <c r="F41" s="20">
-        <f>F$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.2222222222222223E-2</v>
+        <f>ABS(F$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.18</v>
       </c>
       <c r="G41" s="20">
-        <f>G$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.7777777777777776E-2</v>
+        <f>ABS(G$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.1</v>
       </c>
       <c r="H41" s="20">
-        <f>H$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.3333333333333333E-2</v>
+        <f>ABS(H$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>2.0000000000000018E-2</v>
       </c>
       <c r="I41" s="20">
-        <f>I$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>3.8888888888888883E-2</v>
+        <f>ABS(I$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>5.999999999999997E-2</v>
       </c>
       <c r="J41" s="21">
-        <f>J$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.4444444444444439E-2</v>
+        <f>ABS(J$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.13999999999999996</v>
       </c>
       <c r="K41" s="9">
-        <f>K$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>4.9999999999999989E-2</v>
+        <f>ABS(K$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.21999999999999995</v>
       </c>
       <c r="L41" s="9">
-        <f>L$33*(($A41-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.5555555555555546E-2</v>
+        <f>ABS(L$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.29999999999999993</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="6">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="B42" s="11">
-        <f>B$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
+        <f>ABS(B$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.4375</v>
       </c>
       <c r="C42" s="9">
-        <f>C$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.7777777777777792E-3</v>
+        <f>ABS(C$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.36749999999999999</v>
       </c>
       <c r="D42" s="19">
-        <f>D$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>5.5555555555555584E-3</v>
+        <f>ABS(D$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.29749999999999999</v>
       </c>
       <c r="E42" s="20">
-        <f>E$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>8.3333333333333384E-3</v>
+        <f>ABS(E$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.22749999999999995</v>
       </c>
       <c r="F42" s="20">
-        <f>F$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.1111111111111117E-2</v>
+        <f>ABS(F$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.15749999999999997</v>
       </c>
       <c r="G42" s="20">
-        <f>G$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.3888888888888895E-2</v>
+        <f>ABS(G$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="H42" s="20">
-        <f>H$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.6666666666666673E-2</v>
+        <f>ABS(H$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>1.7500000000000016E-2</v>
       </c>
       <c r="I42" s="20">
-        <f>I$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>1.9444444444444452E-2</v>
+        <f>ABS(I$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>5.2499999999999963E-2</v>
       </c>
       <c r="J42" s="21">
-        <f>J$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.222222222222223E-2</v>
+        <f>ABS(J$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.12249999999999994</v>
       </c>
       <c r="K42" s="9">
-        <f>K$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.5000000000000008E-2</v>
+        <f>ABS(K$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.19249999999999992</v>
       </c>
       <c r="L42" s="9">
-        <f>L$33*(($A42-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>2.7777777777777787E-2</v>
+        <f>ABS(L$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.2624999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B43" s="11">
+        <f>ABS(B$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.375</v>
+      </c>
+      <c r="C43" s="9">
+        <f>ABS(C$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.315</v>
+      </c>
+      <c r="D43" s="19">
+        <f>ABS(D$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.255</v>
+      </c>
+      <c r="E43" s="20">
+        <f>ABS(E$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.19499999999999998</v>
+      </c>
+      <c r="F43" s="20">
+        <f>ABS(F$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.13499999999999998</v>
+      </c>
+      <c r="G43" s="20">
+        <f>ABS(G$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H43" s="20">
+        <f>ABS(H$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>1.5000000000000013E-2</v>
+      </c>
+      <c r="I43" s="20">
+        <f>ABS(I$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>4.4999999999999971E-2</v>
+      </c>
+      <c r="J43" s="21">
+        <f>ABS(J$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.10499999999999995</v>
+      </c>
+      <c r="K43" s="9">
+        <f>ABS(K$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.16499999999999995</v>
+      </c>
+      <c r="L43" s="9">
+        <f>ABS(L$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.22499999999999992</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="6">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="B44" s="11">
+        <f>ABS(B$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="C44" s="9">
+        <f>ABS(C$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="D44" s="19">
+        <f>ABS(D$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="E44" s="20">
+        <f>ABS(E$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.16249999999999998</v>
+      </c>
+      <c r="F44" s="20">
+        <f>ABS(F$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.11249999999999999</v>
+      </c>
+      <c r="G44" s="20">
+        <f>ABS(G$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H44" s="20">
+        <f>ABS(H$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>1.2500000000000011E-2</v>
+      </c>
+      <c r="I44" s="20">
+        <f>ABS(I$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>3.7499999999999978E-2</v>
+      </c>
+      <c r="J44" s="21">
+        <f>ABS(J$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>8.7499999999999967E-2</v>
+      </c>
+      <c r="K44" s="9">
+        <f>ABS(K$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.13749999999999996</v>
+      </c>
+      <c r="L44" s="9">
+        <f>ABS(L$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.18749999999999994</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="6">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="B45" s="11">
+        <f>ABS(B$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="C45" s="9">
+        <f>ABS(C$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.20999999999999996</v>
+      </c>
+      <c r="D45" s="19">
+        <f>ABS(D$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.16999999999999996</v>
+      </c>
+      <c r="E45" s="20">
+        <f>ABS(E$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.12999999999999995</v>
+      </c>
+      <c r="F45" s="20">
+        <f>ABS(F$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>8.9999999999999969E-2</v>
+      </c>
+      <c r="G45" s="20">
+        <f>ABS(G$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="H45" s="20">
+        <f>ABS(H$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>1.0000000000000007E-2</v>
+      </c>
+      <c r="I45" s="20">
+        <f>ABS(I$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>2.9999999999999975E-2</v>
+      </c>
+      <c r="J45" s="21">
+        <f>ABS(J$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>6.9999999999999951E-2</v>
+      </c>
+      <c r="K45" s="9">
+        <f>ABS(K$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.10999999999999995</v>
+      </c>
+      <c r="L45" s="9">
+        <f>ABS(L$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.14999999999999991</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="6">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="B46" s="11">
+        <f>ABS(B$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.18750000000000003</v>
+      </c>
+      <c r="C46" s="9">
+        <f>ABS(C$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.15750000000000003</v>
+      </c>
+      <c r="D46" s="19">
+        <f>ABS(D$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.1275</v>
+      </c>
+      <c r="E46" s="20">
+        <f>ABS(E$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="F46" s="20">
+        <f>ABS(F$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="G46" s="20">
+        <f>ABS(G$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>3.7500000000000006E-2</v>
+      </c>
+      <c r="H46" s="20">
+        <f>ABS(H$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>7.5000000000000075E-3</v>
+      </c>
+      <c r="I46" s="20">
+        <f>ABS(I$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>2.2499999999999989E-2</v>
+      </c>
+      <c r="J46" s="21">
+        <f>ABS(J$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>5.2499999999999991E-2</v>
+      </c>
+      <c r="K46" s="9">
+        <f>ABS(K$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>8.249999999999999E-2</v>
+      </c>
+      <c r="L46" s="9">
+        <f>ABS(L$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.11249999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="6">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="B47" s="11">
+        <f>ABS(B$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.12499999999999997</v>
+      </c>
+      <c r="C47" s="9">
+        <f>ABS(C$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>0.10499999999999998</v>
+      </c>
+      <c r="D47" s="19">
+        <f>ABS(D$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>8.4999999999999978E-2</v>
+      </c>
+      <c r="E47" s="20">
+        <f>ABS(E$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>6.4999999999999974E-2</v>
+      </c>
+      <c r="F47" s="20">
+        <f>ABS(F$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>4.4999999999999984E-2</v>
+      </c>
+      <c r="G47" s="20">
+        <f>ABS(G$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="H47" s="20">
+        <f>ABS(H$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>5.0000000000000036E-3</v>
+      </c>
+      <c r="I47" s="20">
+        <f>ABS(I$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>1.4999999999999987E-2</v>
+      </c>
+      <c r="J47" s="21">
+        <f>ABS(J$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>3.4999999999999976E-2</v>
+      </c>
+      <c r="K47" s="9">
+        <f>ABS(K$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>5.4999999999999973E-2</v>
+      </c>
+      <c r="L47" s="9">
+        <f>ABS(L$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>7.4999999999999956E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="6">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B43" s="11">
-        <f>B$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="C43" s="9">
-        <f>C$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="D43" s="22">
-        <f>D$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="23">
-        <f>E$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="F43" s="23">
-        <f>F$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="G43" s="23">
-        <f>G$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="H43" s="23">
-        <f>H$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="I43" s="23">
-        <f>I$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="J43" s="24">
-        <f>J$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="K43" s="9">
-        <f>K$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-      <c r="L43" s="9">
-        <f>L$33*(($A43-'Skill to Value'!$C$3)*(0-$E$15)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L44">
-        <f>_xlfn.VAR.P(B34:L43)</f>
-        <v>3.7905092592592604E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
+      <c r="B48" s="11">
+        <f>ABS(B$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>6.2500000000000056E-2</v>
+      </c>
+      <c r="C48" s="9">
+        <f>ABS(C$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>5.2500000000000047E-2</v>
+      </c>
+      <c r="D48" s="22">
+        <f>ABS(D$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>4.2500000000000038E-2</v>
+      </c>
+      <c r="E48" s="23">
+        <f>ABS(E$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>3.2500000000000022E-2</v>
+      </c>
+      <c r="F48" s="23">
+        <f>ABS(F$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>2.2500000000000017E-2</v>
+      </c>
+      <c r="G48" s="23">
+        <f>ABS(G$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>1.2500000000000011E-2</v>
+      </c>
+      <c r="H48" s="23">
+        <f>ABS(H$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>2.5000000000000044E-3</v>
+      </c>
+      <c r="I48" s="23">
+        <f>ABS(I$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>7.5000000000000023E-3</v>
+      </c>
+      <c r="J48" s="24">
+        <f>ABS(J$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>1.7500000000000009E-2</v>
+      </c>
+      <c r="K48" s="9">
+        <f>ABS(K$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>2.7500000000000014E-2</v>
+      </c>
+      <c r="L48" s="9">
+        <f>ABS(L$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
+        <v>3.7500000000000019E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L49" s="31" t="str">
+        <f>"Var: "&amp;TEXT(_xlfn.VAR.P(B39:L48),"0.00000")</f>
+        <v>Var: 0.01931</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>72</v>
       </c>
-      <c r="B45">
+      <c r="B50">
         <v>1</v>
       </c>
-      <c r="C45">
+      <c r="C50">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B46" s="30">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B51" s="28">
         <v>0.2</v>
       </c>
-      <c r="C46" s="31">
-        <f>(C$45-B$45)*B46</f>
+      <c r="C51" s="29">
+        <f>(C$50-B$50)*B51</f>
         <v>4.8000000000000007</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B47" s="30">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B52" s="28">
         <v>0.8</v>
       </c>
-      <c r="C47" s="31">
-        <f>(C$45-B$45)*B47</f>
+      <c r="C52" s="29">
+        <f>(C$50-B$50)*B52</f>
         <v>19.200000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A49" s="12" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B53" s="33">
+        <f>C53/(C$50-B$50)</f>
+        <v>0.625</v>
+      </c>
+      <c r="C53" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A55" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A53" s="26" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A59" s="40" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B34:L43">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND($A34=ROUNDDOWN($E$14,0),B$33=ROUNDDOWN($E$12,1))</formula>
+  <conditionalFormatting sqref="B39:L48 V23:AE32">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>AND($A23=ROUNDDOWN($E$16,0),B$38=ROUNDDOWN($E$12,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4978,8 +5496,108 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="timingVar">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId5">
+        <control shapeId="1033" r:id="rId4" name="setPassAdjustment">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D28" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>119743</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>22</xdr:col>
+                <xdr:colOff>185057</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>59871</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1033" r:id="rId4" name="setPassAdjustment"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1030" r:id="rId6" name="distance">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D24" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1030" r:id="rId6" name="distance"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1029" r:id="rId8" name="athletePower">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D21" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1029" r:id="rId8" name="athletePower"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId10" name="SpikeSkill">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D16" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId10" name="SpikeSkill"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId12" name="timingVar">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
@@ -4998,132 +5616,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="timingVar"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId6" name="SpikeSkill">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D14" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>27214</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>23</xdr:col>
-                <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId6" name="SpikeSkill"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId8" name="SpikeTimingWindow">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D15" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>27214</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>23</xdr:col>
-                <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId8" name="SpikeTimingWindow"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId10" name="athletePower">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D26" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>27214</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>23</xdr:col>
-                <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1029" r:id="rId10" name="athletePower"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId12" name="distance">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D22" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>27214</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>23</xdr:col>
-                <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1030" r:id="rId12" name="distance"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId14" name="setPassAdjustment">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D20" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>119743</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>22</xdr:col>
-                <xdr:colOff>185057</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>59871</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1033" r:id="rId14" name="setPassAdjustment"/>
+        <control shapeId="1026" r:id="rId12" name="timingVar"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Implemented & Tested Spike calculation adjustments
</commit_message>
<xml_diff>
--- a/Resources/Spike Speed Tracker.xlsx
+++ b/Resources/Spike Speed Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B978A96-8915-417C-99CF-6C7BF5D60B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EB5293-0EA3-4548-8A60-C8D3D26CE003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="96">
   <si>
     <t>Player Skill</t>
   </si>
@@ -279,19 +279,97 @@
   </si>
   <si>
     <t>Spike Skill</t>
+  </si>
+  <si>
+    <t>StoV(s_s,w_s)</t>
+  </si>
+  <si>
+    <t>for spike power = 5, spike skill = 5</t>
+  </si>
+  <si>
+    <t>StoV(p_adj,rng_sp)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</t>
+    </r>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Spike()</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>penalty</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>newTarget</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
+    <t>calc</t>
+  </si>
+  <si>
+    <t>spikeAnim</t>
+  </si>
+  <si>
+    <t>SetSpikeTargetByType()</t>
+  </si>
+  <si>
+    <t>speed m/s</t>
+  </si>
+  <si>
+    <t>speed mph</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +407,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -344,7 +436,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -483,11 +575,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -563,9 +664,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -583,10 +681,22 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,7 +728,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -634,7 +744,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -801,37 +911,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.625</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.52500000000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42499999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32499999999999996</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.22499999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.125</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5000000000000022E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.4999999999999956E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17499999999999993</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.27499999999999991</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.37499999999999989</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -918,37 +1028,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.5625</c:v>
+                  <c:v>6.9444444444444449E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47250000000000003</c:v>
+                  <c:v>5.8333333333333336E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38250000000000001</c:v>
+                  <c:v>4.7222222222222223E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29249999999999998</c:v>
+                  <c:v>3.6111111111111109E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20249999999999999</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1125</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.250000000000002E-2</c:v>
+                  <c:v>2.7777777777777805E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.7499999999999963E-2</c:v>
+                  <c:v>8.3333333333333284E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.15749999999999995</c:v>
+                  <c:v>1.9444444444444437E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.24749999999999991</c:v>
+                  <c:v>3.0555555555555548E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.33749999999999991</c:v>
+                  <c:v>4.1666666666666657E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1035,37 +1145,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>1.388888888888889E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42000000000000004</c:v>
+                  <c:v>1.1666666666666667E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34</c:v>
+                  <c:v>9.4444444444444445E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25999999999999995</c:v>
+                  <c:v>7.2222222222222219E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1</c:v>
+                  <c:v>2.7777777777777779E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0000000000000018E-2</c:v>
+                  <c:v>5.555555555555561E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.999999999999997E-2</c:v>
+                  <c:v>1.6666666666666657E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13999999999999996</c:v>
+                  <c:v>3.8888888888888875E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.21999999999999995</c:v>
+                  <c:v>6.1111111111111097E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.29999999999999993</c:v>
+                  <c:v>8.3333333333333315E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1152,37 +1262,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.4375</c:v>
+                  <c:v>2.0833333333333336E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36749999999999999</c:v>
+                  <c:v>1.7500000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29749999999999999</c:v>
+                  <c:v>1.4166666666666669E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22749999999999995</c:v>
+                  <c:v>1.0833333333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15749999999999997</c:v>
+                  <c:v>7.5000000000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.7499999999999994E-2</c:v>
+                  <c:v>4.1666666666666675E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7500000000000016E-2</c:v>
+                  <c:v>8.3333333333333425E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.2499999999999963E-2</c:v>
+                  <c:v>2.4999999999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12249999999999994</c:v>
+                  <c:v>5.8333333333333319E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19249999999999992</c:v>
+                  <c:v>9.166666666666665E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2624999999999999</c:v>
+                  <c:v>1.2499999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1269,37 +1379,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.375</c:v>
+                  <c:v>2.777777777777778E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.315</c:v>
+                  <c:v>2.3333333333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.255</c:v>
+                  <c:v>1.8888888888888889E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19499999999999998</c:v>
+                  <c:v>1.4444444444444444E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13499999999999998</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.4999999999999997E-2</c:v>
+                  <c:v>5.5555555555555558E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5000000000000013E-2</c:v>
+                  <c:v>1.1111111111111122E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4999999999999971E-2</c:v>
+                  <c:v>3.3333333333333314E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.10499999999999995</c:v>
+                  <c:v>7.777777777777775E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.16499999999999995</c:v>
+                  <c:v>1.2222222222222219E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.22499999999999992</c:v>
+                  <c:v>1.6666666666666663E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1386,37 +1496,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.3125</c:v>
+                  <c:v>3.4722222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26250000000000001</c:v>
+                  <c:v>2.9166666666666667E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21249999999999999</c:v>
+                  <c:v>2.361111111111111E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16249999999999998</c:v>
+                  <c:v>1.805555555555555E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11249999999999999</c:v>
+                  <c:v>1.2499999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2500000000000011E-2</c:v>
+                  <c:v>1.38888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7499999999999978E-2</c:v>
+                  <c:v>4.166666666666664E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.7499999999999967E-2</c:v>
+                  <c:v>9.7222222222222172E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.13749999999999996</c:v>
+                  <c:v>1.5277777777777772E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.18749999999999994</c:v>
+                  <c:v>2.0833333333333325E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1505,37 +1615,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.24999999999999994</c:v>
+                  <c:v>4.1666666666666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20999999999999996</c:v>
+                  <c:v>3.500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16999999999999996</c:v>
+                  <c:v>2.8333333333333339E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12999999999999995</c:v>
+                  <c:v>2.1666666666666667E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9999999999999969E-2</c:v>
+                  <c:v>1.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9999999999999989E-2</c:v>
+                  <c:v>8.333333333333335E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0000000000000007E-2</c:v>
+                  <c:v>1.6666666666666685E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9999999999999975E-2</c:v>
+                  <c:v>4.9999999999999984E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.9999999999999951E-2</c:v>
+                  <c:v>1.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10999999999999995</c:v>
+                  <c:v>1.833333333333333E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14999999999999991</c:v>
+                  <c:v>2.4999999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1624,37 +1734,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.18750000000000003</c:v>
+                  <c:v>4.8611111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15750000000000003</c:v>
+                  <c:v>4.0833333333333333E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1275</c:v>
+                  <c:v>3.3055555555555553E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.7500000000000003E-2</c:v>
+                  <c:v>2.5277777777777774E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.7500000000000004E-2</c:v>
+                  <c:v>1.7499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7500000000000006E-2</c:v>
+                  <c:v>9.7222222222222224E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.5000000000000075E-3</c:v>
+                  <c:v>1.9444444444444461E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2499999999999989E-2</c:v>
+                  <c:v>5.8333333333333301E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.2499999999999991E-2</c:v>
+                  <c:v>1.3611111111111107E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.249999999999999E-2</c:v>
+                  <c:v>2.1388888888888881E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11249999999999999</c:v>
+                  <c:v>2.916666666666666E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1743,37 +1853,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.12499999999999997</c:v>
+                  <c:v>5.5555555555555559E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10499999999999998</c:v>
+                  <c:v>4.6666666666666669E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4999999999999978E-2</c:v>
+                  <c:v>3.7777777777777778E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4999999999999974E-2</c:v>
+                  <c:v>2.8888888888888888E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4999999999999984E-2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4999999999999994E-2</c:v>
+                  <c:v>1.1111111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0000000000000036E-3</c:v>
+                  <c:v>2.2222222222222244E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4999999999999987E-2</c:v>
+                  <c:v>6.6666666666666628E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4999999999999976E-2</c:v>
+                  <c:v>1.555555555555555E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.4999999999999973E-2</c:v>
+                  <c:v>2.4444444444444439E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.4999999999999956E-2</c:v>
+                  <c:v>3.3333333333333326E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1862,37 +1972,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>6.2500000000000056E-2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.2500000000000047E-2</c:v>
+                  <c:v>5.2500000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2500000000000038E-2</c:v>
+                  <c:v>4.2500000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2500000000000022E-2</c:v>
+                  <c:v>3.2499999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2500000000000017E-2</c:v>
+                  <c:v>2.2499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2500000000000011E-2</c:v>
+                  <c:v>1.2500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5000000000000044E-3</c:v>
+                  <c:v>2.5000000000000022E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.5000000000000023E-3</c:v>
+                  <c:v>7.4999999999999963E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7500000000000009E-2</c:v>
+                  <c:v>1.7499999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7500000000000014E-2</c:v>
+                  <c:v>2.7499999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7500000000000019E-2</c:v>
+                  <c:v>3.7499999999999992E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3035,7 +3145,7 @@
           <xdr:col>22</xdr:col>
           <xdr:colOff>185057</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>59870</xdr:rowOff>
+          <xdr:rowOff>59871</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3436,14 +3546,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
@@ -4034,7 +4144,7 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="Q9" s="2">
         <f ca="1">SpikeTime!E24/(SpikeTime!E26*(1-(ABS(SpikeTime!E27)-SpikeTime!E28)))</f>
-        <v>0.19584300085601195</v>
+        <v>0.19482414818159402</v>
       </c>
     </row>
   </sheetData>
@@ -4045,10 +4155,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA744AF-4B66-411A-B034-C8F30C452722}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AE61"/>
+  <dimension ref="A1:AE84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4120,7 +4230,7 @@
       <c r="D12">
         <v>62</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <f>D12/100</f>
         <v>0.62</v>
       </c>
@@ -4181,11 +4291,11 @@
       <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="33">
         <v>0.1</v>
       </c>
-      <c r="E17" s="34">
-        <v>1</v>
+      <c r="E17" s="33">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.4">
@@ -4195,6 +4305,9 @@
       <c r="B18" t="s">
         <v>44</v>
       </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
       <c r="T18" t="s">
         <v>52</v>
       </c>
@@ -4220,7 +4333,7 @@
       </c>
       <c r="E20" s="4">
         <f ca="1">RANDBETWEEN(-E19*100,E19*100)/100</f>
-        <v>0.14000000000000001</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.4">
@@ -4247,47 +4360,47 @@
       </c>
       <c r="E22" s="5">
         <f ca="1">MIN(MAX(E21+E20,1),10)</f>
-        <v>7.14</v>
+        <v>7.24</v>
       </c>
       <c r="U22" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="V22" s="35">
+      <c r="V22" s="34">
         <v>1</v>
       </c>
-      <c r="W22" s="35">
+      <c r="W22" s="34">
         <f>V22+1</f>
         <v>2</v>
       </c>
-      <c r="X22" s="35">
+      <c r="X22" s="34">
         <f t="shared" ref="X22:AE22" si="0">W22+1</f>
         <v>3</v>
       </c>
-      <c r="Y22" s="35">
+      <c r="Y22" s="34">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="Z22" s="35">
+      <c r="Z22" s="34">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="AA22" s="35">
+      <c r="AA22" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="AB22" s="35">
+      <c r="AB22" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="AC22" s="35">
+      <c r="AC22" s="34">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="AD22" s="35">
+      <c r="AD22" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AE22" s="35">
+      <c r="AE22" s="34">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -4301,50 +4414,50 @@
       </c>
       <c r="E23" s="2">
         <f ca="1">E24/(E26*(1-(E27-E28)))</f>
-        <v>0.19584300085601195</v>
+        <v>0.19482414818159402</v>
       </c>
       <c r="U23" s="6">
         <v>1</v>
       </c>
-      <c r="V23" s="36">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.89</v>
-      </c>
-      <c r="W23" s="37">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.885000000000002</v>
-      </c>
-      <c r="X23" s="37">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.88</v>
-      </c>
-      <c r="Y23" s="37">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.875</v>
-      </c>
-      <c r="Z23" s="37">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.87</v>
-      </c>
-      <c r="AA23" s="37">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.864999999999998</v>
-      </c>
-      <c r="AB23" s="37">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.86</v>
-      </c>
-      <c r="AC23" s="37">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.855</v>
-      </c>
-      <c r="AD23" s="37">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.85</v>
-      </c>
-      <c r="AE23" s="37">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.844999999999999</v>
+      <c r="V23" s="35">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>21.989000000000001</v>
+      </c>
+      <c r="W23" s="36">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22.988500000000002</v>
+      </c>
+      <c r="X23" s="36">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23.988</v>
+      </c>
+      <c r="Y23" s="36">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24.987500000000001</v>
+      </c>
+      <c r="Z23" s="36">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25.987000000000002</v>
+      </c>
+      <c r="AA23" s="36">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26.986500000000003</v>
+      </c>
+      <c r="AB23" s="36">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27.986000000000001</v>
+      </c>
+      <c r="AC23" s="36">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28.985500000000002</v>
+      </c>
+      <c r="AD23" s="36">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29.985000000000003</v>
+      </c>
+      <c r="AE23" s="36">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30.984500000000001</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.4">
@@ -4365,45 +4478,45 @@
         <f>U23+1</f>
         <v>2</v>
       </c>
-      <c r="V24" s="38">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.901</v>
-      </c>
-      <c r="W24" s="39">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.8965</v>
-      </c>
-      <c r="X24" s="39">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.892000000000003</v>
-      </c>
-      <c r="Y24" s="39">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.887500000000003</v>
-      </c>
-      <c r="Z24" s="39">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.883000000000003</v>
-      </c>
-      <c r="AA24" s="39">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.878500000000003</v>
-      </c>
-      <c r="AB24" s="39">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.874000000000002</v>
-      </c>
-      <c r="AC24" s="39">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.869500000000002</v>
-      </c>
-      <c r="AD24" s="39">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.865000000000002</v>
-      </c>
-      <c r="AE24" s="39">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.860500000000002</v>
+      <c r="V24" s="37">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>21.990222222222222</v>
+      </c>
+      <c r="W24" s="38">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22.989777777777778</v>
+      </c>
+      <c r="X24" s="38">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23.989333333333335</v>
+      </c>
+      <c r="Y24" s="38">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24.988888888888887</v>
+      </c>
+      <c r="Z24" s="38">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25.988444444444443</v>
+      </c>
+      <c r="AA24" s="38">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26.988</v>
+      </c>
+      <c r="AB24" s="38">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27.987555555555556</v>
+      </c>
+      <c r="AC24" s="38">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28.987111111111112</v>
+      </c>
+      <c r="AD24" s="38">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29.986666666666665</v>
+      </c>
+      <c r="AE24" s="38">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30.986222222222221</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.4">
@@ -4423,98 +4536,98 @@
         <f t="shared" ref="U25:U32" si="1">U24+1</f>
         <v>3</v>
       </c>
-      <c r="V25" s="38">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.911999999999999</v>
-      </c>
-      <c r="W25" s="39">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.908000000000001</v>
-      </c>
-      <c r="X25" s="39">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.904</v>
-      </c>
-      <c r="Y25" s="39">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.9</v>
-      </c>
-      <c r="Z25" s="39">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.896000000000001</v>
-      </c>
-      <c r="AA25" s="39">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.891999999999999</v>
-      </c>
-      <c r="AB25" s="39">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.887999999999998</v>
-      </c>
-      <c r="AC25" s="39">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.884</v>
-      </c>
-      <c r="AD25" s="39">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.88</v>
-      </c>
-      <c r="AE25" s="39">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.876000000000001</v>
+      <c r="V25" s="37">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>21.991444444444443</v>
+      </c>
+      <c r="W25" s="38">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22.991055555555555</v>
+      </c>
+      <c r="X25" s="38">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23.990666666666666</v>
+      </c>
+      <c r="Y25" s="38">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24.990277777777777</v>
+      </c>
+      <c r="Z25" s="38">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25.989888888888888</v>
+      </c>
+      <c r="AA25" s="38">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26.9895</v>
+      </c>
+      <c r="AB25" s="38">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27.989111111111111</v>
+      </c>
+      <c r="AC25" s="38">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28.988722222222222</v>
+      </c>
+      <c r="AD25" s="38">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29.988333333333333</v>
+      </c>
+      <c r="AE25" s="38">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30.987944444444445</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+      <c r="A26" s="42" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="4">
         <f ca="1">(E22-'Skill to Value'!C3)*(E25-D25)/('Skill to Value'!D3-'Skill to Value'!C3)+D25</f>
-        <v>28.14</v>
+        <v>28.240000000000002</v>
       </c>
       <c r="U26" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="V26" s="38">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.923000000000002</v>
-      </c>
-      <c r="W26" s="39">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.919500000000003</v>
-      </c>
-      <c r="X26" s="39">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.916</v>
-      </c>
-      <c r="Y26" s="39">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.912500000000001</v>
-      </c>
-      <c r="Z26" s="39">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.909000000000002</v>
-      </c>
-      <c r="AA26" s="39">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.9055</v>
-      </c>
-      <c r="AB26" s="39">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.902000000000001</v>
-      </c>
-      <c r="AC26" s="39">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.898500000000002</v>
-      </c>
-      <c r="AD26" s="39">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.895000000000003</v>
-      </c>
-      <c r="AE26" s="39">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.891500000000001</v>
+      <c r="V26" s="37">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>21.992666666666668</v>
+      </c>
+      <c r="W26" s="38">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22.992333333333335</v>
+      </c>
+      <c r="X26" s="38">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23.992000000000001</v>
+      </c>
+      <c r="Y26" s="38">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24.991666666666667</v>
+      </c>
+      <c r="Z26" s="38">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25.991333333333333</v>
+      </c>
+      <c r="AA26" s="38">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26.991</v>
+      </c>
+      <c r="AB26" s="38">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27.990666666666669</v>
+      </c>
+      <c r="AC26" s="38">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28.990333333333336</v>
+      </c>
+      <c r="AD26" s="38">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29.990000000000002</v>
+      </c>
+      <c r="AE26" s="38">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30.989666666666668</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.4">
@@ -4526,51 +4639,51 @@
       </c>
       <c r="E27" s="4">
         <f>E14*((E16-'Skill to Value'!C3)*(D17-E17)/('Skill to Value'!D3-'Skill to Value'!C3)+E17)</f>
-        <v>2.0000000000000013E-3</v>
+        <v>3.333333333333337E-4</v>
       </c>
       <c r="U27" s="6">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="V27" s="38">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.934000000000001</v>
-      </c>
-      <c r="W27" s="39">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.931000000000001</v>
-      </c>
-      <c r="X27" s="39">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.928000000000001</v>
-      </c>
-      <c r="Y27" s="39">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.925000000000001</v>
-      </c>
-      <c r="Z27" s="39">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.922000000000001</v>
-      </c>
-      <c r="AA27" s="39">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.919</v>
-      </c>
-      <c r="AB27" s="39">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.916</v>
-      </c>
-      <c r="AC27" s="39">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.913</v>
-      </c>
-      <c r="AD27" s="39">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.91</v>
-      </c>
-      <c r="AE27" s="39">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.907</v>
+      <c r="V27" s="37">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>21.99388888888889</v>
+      </c>
+      <c r="W27" s="38">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22.993611111111111</v>
+      </c>
+      <c r="X27" s="38">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23.993333333333332</v>
+      </c>
+      <c r="Y27" s="38">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24.993055555555554</v>
+      </c>
+      <c r="Z27" s="38">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25.992777777777775</v>
+      </c>
+      <c r="AA27" s="38">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26.9925</v>
+      </c>
+      <c r="AB27" s="38">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27.992222222222221</v>
+      </c>
+      <c r="AC27" s="38">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28.991944444444442</v>
+      </c>
+      <c r="AD27" s="38">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29.991666666666667</v>
+      </c>
+      <c r="AE27" s="38">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30.991388888888888</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.4">
@@ -4594,98 +4707,98 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="V28" s="38">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.945</v>
-      </c>
-      <c r="W28" s="39">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.942500000000003</v>
-      </c>
-      <c r="X28" s="39">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.94</v>
-      </c>
-      <c r="Y28" s="39">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.9375</v>
-      </c>
-      <c r="Z28" s="39">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.935000000000002</v>
-      </c>
-      <c r="AA28" s="39">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.932500000000001</v>
-      </c>
-      <c r="AB28" s="39">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.93</v>
-      </c>
-      <c r="AC28" s="39">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.927500000000002</v>
-      </c>
-      <c r="AD28" s="39">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.925000000000001</v>
-      </c>
-      <c r="AE28" s="39">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.922500000000003</v>
+      <c r="V28" s="37">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>21.995111111111111</v>
+      </c>
+      <c r="W28" s="38">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22.994888888888887</v>
+      </c>
+      <c r="X28" s="38">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23.994666666666667</v>
+      </c>
+      <c r="Y28" s="38">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24.994444444444444</v>
+      </c>
+      <c r="Z28" s="38">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25.994222222222223</v>
+      </c>
+      <c r="AA28" s="38">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26.994</v>
+      </c>
+      <c r="AB28" s="38">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27.993777777777776</v>
+      </c>
+      <c r="AC28" s="38">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28.993555555555556</v>
+      </c>
+      <c r="AD28" s="38">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29.993333333333332</v>
+      </c>
+      <c r="AE28" s="38">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30.993111111111112</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
+      <c r="A29" s="41" t="s">
         <v>77</v>
       </c>
       <c r="E29" s="4">
         <f>(1-(E27-E28))</f>
-        <v>0.998</v>
+        <v>0.9996666666666667</v>
       </c>
       <c r="U29" s="6">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="V29" s="38">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.956</v>
-      </c>
-      <c r="W29" s="39">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.954000000000001</v>
-      </c>
-      <c r="X29" s="39">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.951999999999998</v>
-      </c>
-      <c r="Y29" s="39">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.95</v>
-      </c>
-      <c r="Z29" s="39">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.948</v>
-      </c>
-      <c r="AA29" s="39">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.946000000000002</v>
-      </c>
-      <c r="AB29" s="39">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.943999999999999</v>
-      </c>
-      <c r="AC29" s="39">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.942</v>
-      </c>
-      <c r="AD29" s="39">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.94</v>
-      </c>
-      <c r="AE29" s="39">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.937999999999999</v>
+      <c r="V29" s="37">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>21.996333333333332</v>
+      </c>
+      <c r="W29" s="38">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22.996166666666667</v>
+      </c>
+      <c r="X29" s="38">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23.996000000000002</v>
+      </c>
+      <c r="Y29" s="38">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24.995833333333334</v>
+      </c>
+      <c r="Z29" s="38">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25.995666666666668</v>
+      </c>
+      <c r="AA29" s="38">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26.9955</v>
+      </c>
+      <c r="AB29" s="38">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27.995333333333335</v>
+      </c>
+      <c r="AC29" s="38">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28.995166666666666</v>
+      </c>
+      <c r="AD29" s="38">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29.995000000000001</v>
+      </c>
+      <c r="AE29" s="38">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30.994833333333332</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.4">
@@ -4694,51 +4807,51 @@
       </c>
       <c r="E30" s="25">
         <f ca="1">E26*E29</f>
-        <v>28.08372</v>
+        <v>28.230586666666671</v>
       </c>
       <c r="U30" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="V30" s="38">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.966999999999999</v>
-      </c>
-      <c r="W30" s="39">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.965499999999999</v>
-      </c>
-      <c r="X30" s="39">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.963999999999999</v>
-      </c>
-      <c r="Y30" s="39">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.962499999999999</v>
-      </c>
-      <c r="Z30" s="39">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.960999999999999</v>
-      </c>
-      <c r="AA30" s="39">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.959499999999998</v>
-      </c>
-      <c r="AB30" s="39">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.957999999999998</v>
-      </c>
-      <c r="AC30" s="39">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.956499999999998</v>
-      </c>
-      <c r="AD30" s="39">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.954999999999998</v>
-      </c>
-      <c r="AE30" s="39">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.953499999999998</v>
+      <c r="V30" s="37">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>21.997555555555557</v>
+      </c>
+      <c r="W30" s="38">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22.997444444444447</v>
+      </c>
+      <c r="X30" s="38">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23.997333333333334</v>
+      </c>
+      <c r="Y30" s="38">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24.997222222222224</v>
+      </c>
+      <c r="Z30" s="38">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25.997111111111114</v>
+      </c>
+      <c r="AA30" s="38">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26.997</v>
+      </c>
+      <c r="AB30" s="38">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27.99688888888889</v>
+      </c>
+      <c r="AC30" s="38">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28.99677777777778</v>
+      </c>
+      <c r="AD30" s="38">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29.99666666666667</v>
+      </c>
+      <c r="AE30" s="38">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30.996555555555556</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.4">
@@ -4746,45 +4859,45 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="V31" s="38">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.978000000000002</v>
-      </c>
-      <c r="W31" s="39">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.977</v>
-      </c>
-      <c r="X31" s="39">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.975999999999999</v>
-      </c>
-      <c r="Y31" s="39">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.975000000000001</v>
-      </c>
-      <c r="Z31" s="39">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.974</v>
-      </c>
-      <c r="AA31" s="39">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.972999999999999</v>
-      </c>
-      <c r="AB31" s="39">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.972000000000001</v>
-      </c>
-      <c r="AC31" s="39">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.971</v>
-      </c>
-      <c r="AD31" s="39">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.97</v>
-      </c>
-      <c r="AE31" s="39">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.969000000000001</v>
+      <c r="V31" s="37">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>21.998777777777779</v>
+      </c>
+      <c r="W31" s="38">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22.99872222222222</v>
+      </c>
+      <c r="X31" s="38">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23.998666666666665</v>
+      </c>
+      <c r="Y31" s="38">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24.99861111111111</v>
+      </c>
+      <c r="Z31" s="38">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25.998555555555555</v>
+      </c>
+      <c r="AA31" s="38">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26.9985</v>
+      </c>
+      <c r="AB31" s="38">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27.998444444444445</v>
+      </c>
+      <c r="AC31" s="38">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28.998388888888886</v>
+      </c>
+      <c r="AD31" s="38">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29.998333333333331</v>
+      </c>
+      <c r="AE31" s="38">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30.998277777777776</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.4">
@@ -4793,7 +4906,7 @@
       </c>
       <c r="E32" s="25">
         <f ca="1">E24/E23</f>
-        <v>28.08372</v>
+        <v>28.230586666666671</v>
       </c>
       <c r="F32" t="s">
         <v>71</v>
@@ -4802,62 +4915,89 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="V32" s="38">
-        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>21.988999999999997</v>
-      </c>
-      <c r="W32" s="39">
-        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>22.988499999999998</v>
-      </c>
-      <c r="X32" s="39">
-        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>23.988</v>
-      </c>
-      <c r="Y32" s="39">
-        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>24.987499999999997</v>
-      </c>
-      <c r="Z32" s="39">
-        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>25.986999999999998</v>
-      </c>
-      <c r="AA32" s="39">
-        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>26.986499999999999</v>
-      </c>
-      <c r="AB32" s="39">
-        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>27.985999999999997</v>
-      </c>
-      <c r="AC32" s="39">
-        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>28.985499999999998</v>
-      </c>
-      <c r="AD32" s="39">
-        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>29.984999999999999</v>
-      </c>
-      <c r="AE32" s="39">
-        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)-$E$28))</f>
-        <v>30.984499999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="V32" s="37">
+        <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>22</v>
+      </c>
+      <c r="W32" s="38">
+        <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>23</v>
+      </c>
+      <c r="X32" s="38">
+        <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>24</v>
+      </c>
+      <c r="Y32" s="38">
+        <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>25</v>
+      </c>
+      <c r="Z32" s="38">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>26</v>
+      </c>
+      <c r="AA32" s="38">
+        <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>27</v>
+      </c>
+      <c r="AB32" s="38">
+        <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>28</v>
+      </c>
+      <c r="AC32" s="38">
+        <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>29</v>
+      </c>
+      <c r="AD32" s="38">
+        <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>30</v>
+      </c>
+      <c r="AE32" s="38">
+        <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U32-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>66</v>
       </c>
       <c r="E33" s="25">
         <f ca="1">E32*2.23694</f>
-        <v>62.821596616800001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
+        <v>63.150128538133345</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="U34" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y34" s="25">
+        <f>Z27</f>
+        <v>25.992777777777775</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="U35" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y35" s="25">
+        <f>(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)</f>
+        <v>5.5555555555555559E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="U36" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y36" s="25">
+        <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>63</v>
       </c>
@@ -4904,510 +5044,513 @@
         <f t="shared" si="2"/>
         <v>0.99999999999999989</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="U38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="6">
         <v>1</v>
       </c>
       <c r="B39" s="10">
         <f>ABS(B$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="C39" s="8">
         <f>ABS(C$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.52500000000000002</v>
+        <v>0</v>
       </c>
       <c r="D39" s="16">
         <f>ABS(D$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.42499999999999999</v>
+        <v>0</v>
       </c>
       <c r="E39" s="17">
         <f>ABS(E$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.32499999999999996</v>
+        <v>0</v>
       </c>
       <c r="F39" s="17">
         <f>ABS(F$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.22499999999999998</v>
+        <v>0</v>
       </c>
       <c r="G39" s="17">
         <f>ABS(G$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="H39" s="17">
         <f>ABS(H$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>2.5000000000000022E-2</v>
+        <v>0</v>
       </c>
       <c r="I39" s="17">
         <f>ABS(I$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>7.4999999999999956E-2</v>
+        <v>0</v>
       </c>
       <c r="J39" s="18">
         <f>ABS(J$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.17499999999999993</v>
+        <v>0</v>
       </c>
       <c r="K39" s="8">
         <f>ABS(K$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.27499999999999991</v>
+        <v>0</v>
       </c>
       <c r="L39" s="8">
         <f>ABS(L$38-$E$13)*(($A39-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.37499999999999989</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="6">
         <f>A39+1</f>
         <v>2</v>
       </c>
       <c r="B40" s="11">
         <f>ABS(B$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.5625</v>
+        <v>6.9444444444444449E-3</v>
       </c>
       <c r="C40" s="9">
         <f>ABS(C$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.47250000000000003</v>
+        <v>5.8333333333333336E-3</v>
       </c>
       <c r="D40" s="19">
         <f>ABS(D$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.38250000000000001</v>
+        <v>4.7222222222222223E-3</v>
       </c>
       <c r="E40" s="20">
         <f>ABS(E$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.29249999999999998</v>
+        <v>3.6111111111111109E-3</v>
       </c>
       <c r="F40" s="20">
         <f>ABS(F$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.20249999999999999</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="G40" s="20">
         <f>ABS(G$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.1125</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="H40" s="20">
         <f>ABS(H$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>2.250000000000002E-2</v>
+        <v>2.7777777777777805E-4</v>
       </c>
       <c r="I40" s="20">
         <f>ABS(I$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>6.7499999999999963E-2</v>
+        <v>8.3333333333333284E-4</v>
       </c>
       <c r="J40" s="21">
         <f>ABS(J$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.15749999999999995</v>
+        <v>1.9444444444444437E-3</v>
       </c>
       <c r="K40" s="9">
         <f>ABS(K$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.24749999999999991</v>
+        <v>3.0555555555555548E-3</v>
       </c>
       <c r="L40" s="9">
         <f>ABS(L$38-$E$13)*(($A40-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.33749999999999991</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>4.1666666666666657E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="6">
         <f t="shared" ref="A41:A48" si="3">A40+1</f>
         <v>3</v>
       </c>
       <c r="B41" s="11">
         <f>ABS(B$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.5</v>
+        <v>1.388888888888889E-2</v>
       </c>
       <c r="C41" s="9">
         <f>ABS(C$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.42000000000000004</v>
+        <v>1.1666666666666667E-2</v>
       </c>
       <c r="D41" s="19">
         <f>ABS(D$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.34</v>
+        <v>9.4444444444444445E-3</v>
       </c>
       <c r="E41" s="20">
         <f>ABS(E$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.25999999999999995</v>
+        <v>7.2222222222222219E-3</v>
       </c>
       <c r="F41" s="20">
         <f>ABS(F$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.18</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G41" s="20">
         <f>ABS(G$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.1</v>
+        <v>2.7777777777777779E-3</v>
       </c>
       <c r="H41" s="20">
         <f>ABS(H$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>2.0000000000000018E-2</v>
+        <v>5.555555555555561E-4</v>
       </c>
       <c r="I41" s="20">
         <f>ABS(I$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>5.999999999999997E-2</v>
+        <v>1.6666666666666657E-3</v>
       </c>
       <c r="J41" s="21">
         <f>ABS(J$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.13999999999999996</v>
+        <v>3.8888888888888875E-3</v>
       </c>
       <c r="K41" s="9">
         <f>ABS(K$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.21999999999999995</v>
+        <v>6.1111111111111097E-3</v>
       </c>
       <c r="L41" s="9">
         <f>ABS(L$38-$E$13)*(($A41-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.29999999999999993</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>8.3333333333333315E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="6">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B42" s="11">
         <f>ABS(B$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.4375</v>
+        <v>2.0833333333333336E-2</v>
       </c>
       <c r="C42" s="9">
         <f>ABS(C$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.36749999999999999</v>
+        <v>1.7500000000000005E-2</v>
       </c>
       <c r="D42" s="19">
         <f>ABS(D$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.29749999999999999</v>
+        <v>1.4166666666666669E-2</v>
       </c>
       <c r="E42" s="20">
         <f>ABS(E$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.22749999999999995</v>
+        <v>1.0833333333333334E-2</v>
       </c>
       <c r="F42" s="20">
         <f>ABS(F$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.15749999999999997</v>
+        <v>7.5000000000000006E-3</v>
       </c>
       <c r="G42" s="20">
         <f>ABS(G$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>8.7499999999999994E-2</v>
+        <v>4.1666666666666675E-3</v>
       </c>
       <c r="H42" s="20">
         <f>ABS(H$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>1.7500000000000016E-2</v>
+        <v>8.3333333333333425E-4</v>
       </c>
       <c r="I42" s="20">
         <f>ABS(I$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>5.2499999999999963E-2</v>
+        <v>2.4999999999999992E-3</v>
       </c>
       <c r="J42" s="21">
         <f>ABS(J$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.12249999999999994</v>
+        <v>5.8333333333333319E-3</v>
       </c>
       <c r="K42" s="9">
         <f>ABS(K$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.19249999999999992</v>
+        <v>9.166666666666665E-3</v>
       </c>
       <c r="L42" s="9">
         <f>ABS(L$38-$E$13)*(($A42-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.2624999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="6">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B43" s="11">
         <f>ABS(B$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.375</v>
+        <v>2.777777777777778E-2</v>
       </c>
       <c r="C43" s="9">
         <f>ABS(C$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.315</v>
+        <v>2.3333333333333334E-2</v>
       </c>
       <c r="D43" s="19">
         <f>ABS(D$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.255</v>
+        <v>1.8888888888888889E-2</v>
       </c>
       <c r="E43" s="20">
         <f>ABS(E$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.19499999999999998</v>
+        <v>1.4444444444444444E-2</v>
       </c>
       <c r="F43" s="20">
         <f>ABS(F$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.13499999999999998</v>
+        <v>0.01</v>
       </c>
       <c r="G43" s="20">
         <f>ABS(G$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>7.4999999999999997E-2</v>
+        <v>5.5555555555555558E-3</v>
       </c>
       <c r="H43" s="20">
         <f>ABS(H$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>1.5000000000000013E-2</v>
+        <v>1.1111111111111122E-3</v>
       </c>
       <c r="I43" s="20">
         <f>ABS(I$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>4.4999999999999971E-2</v>
+        <v>3.3333333333333314E-3</v>
       </c>
       <c r="J43" s="21">
         <f>ABS(J$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.10499999999999995</v>
+        <v>7.777777777777775E-3</v>
       </c>
       <c r="K43" s="9">
         <f>ABS(K$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.16499999999999995</v>
+        <v>1.2222222222222219E-2</v>
       </c>
       <c r="L43" s="9">
         <f>ABS(L$38-$E$13)*(($A43-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.22499999999999992</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1.6666666666666663E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="6">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B44" s="11">
         <f>ABS(B$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.3125</v>
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="C44" s="9">
         <f>ABS(C$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.26250000000000001</v>
+        <v>2.9166666666666667E-2</v>
       </c>
       <c r="D44" s="19">
         <f>ABS(D$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.21249999999999999</v>
+        <v>2.361111111111111E-2</v>
       </c>
       <c r="E44" s="20">
         <f>ABS(E$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.16249999999999998</v>
+        <v>1.805555555555555E-2</v>
       </c>
       <c r="F44" s="20">
         <f>ABS(F$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.11249999999999999</v>
+        <v>1.2499999999999997E-2</v>
       </c>
       <c r="G44" s="20">
         <f>ABS(G$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>6.25E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="H44" s="20">
         <f>ABS(H$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>1.2500000000000011E-2</v>
+        <v>1.38888888888889E-3</v>
       </c>
       <c r="I44" s="20">
         <f>ABS(I$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>3.7499999999999978E-2</v>
+        <v>4.166666666666664E-3</v>
       </c>
       <c r="J44" s="21">
         <f>ABS(J$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>8.7499999999999967E-2</v>
+        <v>9.7222222222222172E-3</v>
       </c>
       <c r="K44" s="9">
         <f>ABS(K$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.13749999999999996</v>
+        <v>1.5277777777777772E-2</v>
       </c>
       <c r="L44" s="9">
         <f>ABS(L$38-$E$13)*(($A44-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.18749999999999994</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>2.0833333333333325E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="6">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B45" s="11">
         <f>ABS(B$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.24999999999999994</v>
+        <v>4.1666666666666671E-2</v>
       </c>
       <c r="C45" s="9">
         <f>ABS(C$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.20999999999999996</v>
+        <v>3.500000000000001E-2</v>
       </c>
       <c r="D45" s="19">
         <f>ABS(D$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.16999999999999996</v>
+        <v>2.8333333333333339E-2</v>
       </c>
       <c r="E45" s="20">
         <f>ABS(E$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.12999999999999995</v>
+        <v>2.1666666666666667E-2</v>
       </c>
       <c r="F45" s="20">
         <f>ABS(F$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>8.9999999999999969E-2</v>
+        <v>1.5000000000000001E-2</v>
       </c>
       <c r="G45" s="20">
         <f>ABS(G$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>4.9999999999999989E-2</v>
+        <v>8.333333333333335E-3</v>
       </c>
       <c r="H45" s="20">
         <f>ABS(H$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>1.0000000000000007E-2</v>
+        <v>1.6666666666666685E-3</v>
       </c>
       <c r="I45" s="20">
         <f>ABS(I$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>2.9999999999999975E-2</v>
+        <v>4.9999999999999984E-3</v>
       </c>
       <c r="J45" s="21">
         <f>ABS(J$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>6.9999999999999951E-2</v>
+        <v>1.1666666666666664E-2</v>
       </c>
       <c r="K45" s="9">
         <f>ABS(K$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.10999999999999995</v>
+        <v>1.833333333333333E-2</v>
       </c>
       <c r="L45" s="9">
         <f>ABS(L$38-$E$13)*(($A45-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.14999999999999991</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>2.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="6">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B46" s="11">
         <f>ABS(B$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.18750000000000003</v>
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="C46" s="9">
         <f>ABS(C$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.15750000000000003</v>
+        <v>4.0833333333333333E-2</v>
       </c>
       <c r="D46" s="19">
         <f>ABS(D$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.1275</v>
+        <v>3.3055555555555553E-2</v>
       </c>
       <c r="E46" s="20">
         <f>ABS(E$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>9.7500000000000003E-2</v>
+        <v>2.5277777777777774E-2</v>
       </c>
       <c r="F46" s="20">
         <f>ABS(F$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>6.7500000000000004E-2</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="G46" s="20">
         <f>ABS(G$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>3.7500000000000006E-2</v>
+        <v>9.7222222222222224E-3</v>
       </c>
       <c r="H46" s="20">
         <f>ABS(H$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>7.5000000000000075E-3</v>
+        <v>1.9444444444444461E-3</v>
       </c>
       <c r="I46" s="20">
         <f>ABS(I$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>2.2499999999999989E-2</v>
+        <v>5.8333333333333301E-3</v>
       </c>
       <c r="J46" s="21">
         <f>ABS(J$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>5.2499999999999991E-2</v>
+        <v>1.3611111111111107E-2</v>
       </c>
       <c r="K46" s="9">
         <f>ABS(K$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>8.249999999999999E-2</v>
+        <v>2.1388888888888881E-2</v>
       </c>
       <c r="L46" s="9">
         <f>ABS(L$38-$E$13)*(($A46-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.11249999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>2.916666666666666E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="6">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B47" s="11">
         <f>ABS(B$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.12499999999999997</v>
+        <v>5.5555555555555559E-2</v>
       </c>
       <c r="C47" s="9">
         <f>ABS(C$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>0.10499999999999998</v>
+        <v>4.6666666666666669E-2</v>
       </c>
       <c r="D47" s="19">
         <f>ABS(D$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>8.4999999999999978E-2</v>
+        <v>3.7777777777777778E-2</v>
       </c>
       <c r="E47" s="20">
         <f>ABS(E$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>6.4999999999999974E-2</v>
+        <v>2.8888888888888888E-2</v>
       </c>
       <c r="F47" s="20">
         <f>ABS(F$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>4.4999999999999984E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G47" s="20">
         <f>ABS(G$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>2.4999999999999994E-2</v>
+        <v>1.1111111111111112E-2</v>
       </c>
       <c r="H47" s="20">
         <f>ABS(H$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>5.0000000000000036E-3</v>
+        <v>2.2222222222222244E-3</v>
       </c>
       <c r="I47" s="20">
         <f>ABS(I$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>1.4999999999999987E-2</v>
+        <v>6.6666666666666628E-3</v>
       </c>
       <c r="J47" s="21">
         <f>ABS(J$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>3.4999999999999976E-2</v>
+        <v>1.555555555555555E-2</v>
       </c>
       <c r="K47" s="9">
         <f>ABS(K$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>5.4999999999999973E-2</v>
+        <v>2.4444444444444439E-2</v>
       </c>
       <c r="L47" s="9">
         <f>ABS(L$38-$E$13)*(($A47-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>7.4999999999999956E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>3.3333333333333326E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="6">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B48" s="11">
         <f>ABS(B$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>6.2500000000000056E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C48" s="9">
         <f>ABS(C$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>5.2500000000000047E-2</v>
+        <v>5.2500000000000005E-2</v>
       </c>
       <c r="D48" s="22">
         <f>ABS(D$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>4.2500000000000038E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="E48" s="23">
         <f>ABS(E$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>3.2500000000000022E-2</v>
+        <v>3.2499999999999994E-2</v>
       </c>
       <c r="F48" s="23">
         <f>ABS(F$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>2.2500000000000017E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="G48" s="23">
         <f>ABS(G$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>1.2500000000000011E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="H48" s="23">
         <f>ABS(H$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>2.5000000000000044E-3</v>
+        <v>2.5000000000000022E-3</v>
       </c>
       <c r="I48" s="23">
         <f>ABS(I$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>7.5000000000000023E-3</v>
+        <v>7.4999999999999963E-3</v>
       </c>
       <c r="J48" s="24">
         <f>ABS(J$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>1.7500000000000009E-2</v>
+        <v>1.7499999999999995E-2</v>
       </c>
       <c r="K48" s="9">
         <f>ABS(K$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>2.7500000000000014E-2</v>
+        <v>2.7499999999999993E-2</v>
       </c>
       <c r="L48" s="9">
         <f>ABS(L$38-$E$13)*(($A48-'Skill to Value'!$C$3)*($D$17-$E$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$E$17)</f>
-        <v>3.7500000000000019E-2</v>
+        <v>3.7499999999999992E-2</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L49" s="31" t="str">
+      <c r="L49" s="30" t="str">
         <f>"Var: "&amp;TEXT(_xlfn.VAR.P(B39:L48),"0.00000")</f>
-        <v>Var: 0.01931</v>
+        <v>Var: 0.00020</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.4">
@@ -5440,7 +5583,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B53" s="33">
+      <c r="B53" s="32">
         <f>C53/(C$50-B$50)</f>
         <v>0.625</v>
       </c>
@@ -5469,7 +5612,7 @@
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A59" s="40" t="s">
+      <c r="A59" s="39" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5481,6 +5624,187 @@
     <row r="61" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A64" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A65" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A66" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B66" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C66" s="45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A67" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B67" s="46">
+        <v>0.43637880000000001</v>
+      </c>
+      <c r="C67" s="46"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A68" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68">
+        <v>0.18862119999999999</v>
+      </c>
+      <c r="C68">
+        <f>E13-B67</f>
+        <v>0.18862119999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A69" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69">
+        <v>3.3333340000000003E-2</v>
+      </c>
+      <c r="C69">
+        <f>((B65-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)</f>
+        <v>3.3333333333333326E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A70" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70">
+        <v>1.886212</v>
+      </c>
+      <c r="C70">
+        <f>B68*E18</f>
+        <v>1.886212</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A71" s="43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A72" s="43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A76" s="45"/>
+      <c r="B76" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A77" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77">
+        <v>8.6725379999999994</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A78" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78">
+        <v>-0.59661379999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A79" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>27.403390000000002</v>
+      </c>
+      <c r="C79" s="49">
+        <f>(MIN(MAX(B74+B78,1),10)-'Skill to Value'!C3)*(E25-D25)/('Skill to Value'!D3-'Skill to Value'!C3)+D25</f>
+        <v>27.4033862</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A80" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80">
+        <v>7.2634489999999999E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A81" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A82" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82">
+        <v>0.31879239999999998</v>
+      </c>
+      <c r="C82">
+        <f>B77/(C79*(1-(B80-B81)))</f>
+        <v>0.31879240632689365</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A83" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="4">
+        <v>27.2</v>
+      </c>
+      <c r="C83" s="4">
+        <f>B77/C82</f>
+        <v>27.204343101908997</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A84" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84">
+        <v>60.85</v>
+      </c>
+      <c r="C84" s="4">
+        <f>C83*2.23694</f>
+        <v>60.854483258384313</v>
       </c>
     </row>
   </sheetData>
@@ -5496,44 +5820,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId4" name="setPassAdjustment">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D28" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>119743</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>22</xdr:col>
-                <xdr:colOff>185057</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>59871</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1033" r:id="rId4" name="setPassAdjustment"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId6" name="distance">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D24" r:id="rId7">
+        <control shapeId="1026" r:id="rId4" name="timingVar">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
                 <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>9</xdr:row>
                 <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>23</xdr:col>
                 <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>9</xdr:row>
                 <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
@@ -5541,7 +5840,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId6" name="distance"/>
+        <control shapeId="1026" r:id="rId4" name="timingVar"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId6" name="SpikeSkill">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D16" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId6" name="SpikeSkill"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -5571,19 +5895,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId10" name="SpikeSkill">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D16" r:id="rId11">
+        <control shapeId="1030" r:id="rId10" name="distance">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D24" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
                 <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>11</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>23</xdr:col>
                 <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>11</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
@@ -5591,32 +5915,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId10" name="SpikeSkill"/>
+        <control shapeId="1030" r:id="rId10" name="distance"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId12" name="timingVar">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId13">
+        <control shapeId="1033" r:id="rId12" name="setPassAdjustment">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D28" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
-                <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>27214</xdr:rowOff>
+                <xdr:colOff>119743</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>23</xdr:col>
-                <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
+                <xdr:col>22</xdr:col>
+                <xdr:colOff>185057</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>59871</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId12" name="timingVar"/>
+        <control shapeId="1033" r:id="rId12" name="setPassAdjustment"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Adding range from function calls when spike collider is available during animation
</commit_message>
<xml_diff>
--- a/Resources/Spike Speed Tracker.xlsx
+++ b/Resources/Spike Speed Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EB5293-0EA3-4548-8A60-C8D3D26CE003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20255AB7-C714-42E8-AEA3-9643A0A9867A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="105">
   <si>
     <t>Player Skill</t>
   </si>
@@ -356,6 +356,33 @@
   </si>
   <si>
     <t>speed mph</t>
+  </si>
+  <si>
+    <t>OMG Duh</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>spikeTrigger</t>
+  </si>
+  <si>
+    <t>Time in Animation</t>
+  </si>
+  <si>
+    <t>OnJumpEvent</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>OnJumpPeakEvent</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>so is this the range?</t>
   </si>
 </sst>
 </file>
@@ -588,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -685,18 +712,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +750,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -744,7 +766,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3546,14 +3568,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
@@ -4144,7 +4166,7 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="Q9" s="2">
         <f ca="1">SpikeTime!E24/(SpikeTime!E26*(1-(ABS(SpikeTime!E27)-SpikeTime!E28)))</f>
-        <v>0.19482414818159402</v>
+        <v>0.19977610547016036</v>
       </c>
     </row>
   </sheetData>
@@ -4155,10 +4177,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA744AF-4B66-411A-B034-C8F30C452722}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AE84"/>
+  <dimension ref="A1:AE90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4333,7 +4355,7 @@
       </c>
       <c r="E20" s="4">
         <f ca="1">RANDBETWEEN(-E19*100,E19*100)/100</f>
-        <v>0.24</v>
+        <v>-0.46</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.4">
@@ -4360,7 +4382,7 @@
       </c>
       <c r="E22" s="5">
         <f ca="1">MIN(MAX(E21+E20,1),10)</f>
-        <v>7.24</v>
+        <v>6.54</v>
       </c>
       <c r="U22" s="6" t="s">
         <v>79</v>
@@ -4414,7 +4436,7 @@
       </c>
       <c r="E23" s="2">
         <f ca="1">E24/(E26*(1-(E27-E28)))</f>
-        <v>0.19482414818159402</v>
+        <v>0.19977610547016036</v>
       </c>
       <c r="U23" s="6">
         <v>1</v>
@@ -4578,12 +4600,12 @@
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="41" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="4">
         <f ca="1">(E22-'Skill to Value'!C3)*(E25-D25)/('Skill to Value'!D3-'Skill to Value'!C3)+D25</f>
-        <v>28.240000000000002</v>
+        <v>27.54</v>
       </c>
       <c r="U26" s="6">
         <f t="shared" si="1"/>
@@ -4749,7 +4771,7 @@
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="40" t="s">
         <v>77</v>
       </c>
       <c r="E29" s="4">
@@ -4807,7 +4829,7 @@
       </c>
       <c r="E30" s="25">
         <f ca="1">E26*E29</f>
-        <v>28.230586666666671</v>
+        <v>27.530819999999999</v>
       </c>
       <c r="U30" s="6">
         <f t="shared" si="1"/>
@@ -4906,7 +4928,7 @@
       </c>
       <c r="E32" s="25">
         <f ca="1">E24/E23</f>
-        <v>28.230586666666671</v>
+        <v>27.530819999999999</v>
       </c>
       <c r="F32" t="s">
         <v>71</v>
@@ -4962,7 +4984,7 @@
       </c>
       <c r="E33" s="25">
         <f ca="1">E32*2.23694</f>
-        <v>63.150128538133345</v>
+        <v>61.584792490799998</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.4">
@@ -5632,7 +5654,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A65" s="43" t="s">
+      <c r="A65" t="s">
         <v>20</v>
       </c>
       <c r="B65">
@@ -5640,27 +5662,26 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A66" s="44" t="s">
+      <c r="A66" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B66" s="45" t="s">
+      <c r="B66" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="C66" s="45" t="s">
+      <c r="C66" s="42" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A67" s="47" t="s">
+      <c r="A67" t="s">
         <v>92</v>
       </c>
-      <c r="B67" s="46">
+      <c r="B67">
         <v>0.43637880000000001</v>
       </c>
-      <c r="C67" s="46"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A68" s="43" t="s">
+      <c r="A68" t="s">
         <v>38</v>
       </c>
       <c r="B68">
@@ -5672,7 +5693,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A69" s="43" t="s">
+      <c r="A69" t="s">
         <v>86</v>
       </c>
       <c r="B69">
@@ -5684,7 +5705,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A70" s="43" t="s">
+      <c r="A70" t="s">
         <v>87</v>
       </c>
       <c r="B70">
@@ -5696,12 +5717,12 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A71" s="43" t="s">
+      <c r="A71" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A72" s="43" t="s">
+      <c r="A72" t="s">
         <v>89</v>
       </c>
     </row>
@@ -5719,16 +5740,16 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A76" s="45"/>
-      <c r="B76" s="45" t="s">
+      <c r="A76" s="42"/>
+      <c r="B76" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="C76" s="45" t="s">
+      <c r="C76" s="42" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A77" s="48" t="s">
+      <c r="A77" t="s">
         <v>12</v>
       </c>
       <c r="B77">
@@ -5736,7 +5757,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A78" s="48" t="s">
+      <c r="A78" t="s">
         <v>13</v>
       </c>
       <c r="B78">
@@ -5744,19 +5765,19 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A79" s="48" t="s">
+      <c r="A79" t="s">
         <v>14</v>
       </c>
       <c r="B79">
         <v>27.403390000000002</v>
       </c>
-      <c r="C79" s="49">
+      <c r="C79" s="43">
         <f>(MIN(MAX(B74+B78,1),10)-'Skill to Value'!C3)*(E25-D25)/('Skill to Value'!D3-'Skill to Value'!C3)+D25</f>
         <v>27.4033862</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A80" s="48" t="s">
+      <c r="A80" t="s">
         <v>15</v>
       </c>
       <c r="B80">
@@ -5764,7 +5785,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A81" s="48" t="s">
+      <c r="A81" t="s">
         <v>16</v>
       </c>
       <c r="B81">
@@ -5772,7 +5793,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A82" s="48" t="s">
+      <c r="A82" t="s">
         <v>17</v>
       </c>
       <c r="B82">
@@ -5784,7 +5805,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A83" s="48" t="s">
+      <c r="A83" t="s">
         <v>94</v>
       </c>
       <c r="B83" s="4">
@@ -5796,7 +5817,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A84" s="48" t="s">
+      <c r="A84" t="s">
         <v>95</v>
       </c>
       <c r="B84">
@@ -5807,8 +5828,51 @@
         <v>60.854483258384313</v>
       </c>
     </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A86" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
+        <v>97</v>
+      </c>
+      <c r="B87" t="s">
+        <v>98</v>
+      </c>
+      <c r="C87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>100</v>
+      </c>
+      <c r="B88" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" t="s">
+        <v>103</v>
+      </c>
+      <c r="C89">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A90" s="39" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B39:L48 V23:AE32">
+  <conditionalFormatting sqref="V23:AE32 B39:L48">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>AND($A23=ROUNDDOWN($E$16,0),B$38=ROUNDDOWN($E$12,1))</formula>
     </cfRule>
@@ -5820,19 +5884,44 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="timingVar">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId5">
+        <control shapeId="1033" r:id="rId4" name="setPassAdjustment">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D28" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>119743</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>22</xdr:col>
+                <xdr:colOff>185057</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>59871</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1033" r:id="rId4" name="setPassAdjustment"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1030" r:id="rId6" name="distance">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D24" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
                 <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>23</xdr:col>
                 <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
@@ -5840,32 +5929,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="timingVar"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId6" name="SpikeSkill">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D16" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>27214</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>23</xdr:col>
-                <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId6" name="SpikeSkill"/>
+        <control shapeId="1030" r:id="rId6" name="distance"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -5895,19 +5959,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId10" name="distance">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D24" r:id="rId11">
+        <control shapeId="1027" r:id="rId10" name="SpikeSkill">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D16" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
                 <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>11</xdr:row>
                 <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>23</xdr:col>
                 <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>11</xdr:row>
                 <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
@@ -5915,32 +5979,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId10" name="distance"/>
+        <control shapeId="1027" r:id="rId10" name="SpikeSkill"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId12" name="setPassAdjustment">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D28" r:id="rId13">
+        <control shapeId="1026" r:id="rId12" name="timingVar">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
-                <xdr:colOff>119743</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>22</xdr:col>
-                <xdr:colOff>185057</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>59871</xdr:rowOff>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1033" r:id="rId12" name="setPassAdjustment"/>
+        <control shapeId="1026" r:id="rId12" name="timingVar"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Question about range timeline
</commit_message>
<xml_diff>
--- a/Resources/Spike Speed Tracker.xlsx
+++ b/Resources/Spike Speed Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20255AB7-C714-42E8-AEA3-9643A0A9867A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512C94E4-CF5A-4E94-BE7E-4B576B8C1416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{488066F8-1B0E-4D1C-ABA5-8DB35EC8884A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
   <si>
     <t>Player Skill</t>
   </si>
@@ -383,6 +383,12 @@
   </si>
   <si>
     <t>so is this the range?</t>
+  </si>
+  <si>
+    <t>Also!  If the jump peak is when the thing turns off, that's the ideal range</t>
+  </si>
+  <si>
+    <t>but maybe it should be set to enable longer (missed)</t>
   </si>
 </sst>
 </file>
@@ -750,7 +756,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -766,7 +772,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{DFD181E0-5E2F-11CE-A449-00AA004A803D}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D40-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4166,7 +4172,7 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="Q9" s="2">
         <f ca="1">SpikeTime!E24/(SpikeTime!E26*(1-(ABS(SpikeTime!E27)-SpikeTime!E28)))</f>
-        <v>0.19977610547016036</v>
+        <v>0.19235970565467586</v>
       </c>
     </row>
   </sheetData>
@@ -4177,10 +4183,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA744AF-4B66-411A-B034-C8F30C452722}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AE90"/>
+  <dimension ref="A1:AE92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4250,11 +4256,11 @@
         <v>38</v>
       </c>
       <c r="D12">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E12" s="31">
         <f>D12/100</f>
-        <v>0.62</v>
+        <v>0.65</v>
       </c>
       <c r="T12" t="s">
         <v>43</v>
@@ -4274,7 +4280,7 @@
       </c>
       <c r="E14" s="4">
         <f>ABS(E12-E13)</f>
-        <v>5.0000000000000044E-3</v>
+        <v>2.5000000000000022E-2</v>
       </c>
       <c r="T14" t="s">
         <v>11</v>
@@ -4355,7 +4361,7 @@
       </c>
       <c r="E20" s="4">
         <f ca="1">RANDBETWEEN(-E19*100,E19*100)/100</f>
-        <v>-0.46</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.4">
@@ -4382,7 +4388,7 @@
       </c>
       <c r="E22" s="5">
         <f ca="1">MIN(MAX(E21+E20,1),10)</f>
-        <v>6.54</v>
+        <v>7.64</v>
       </c>
       <c r="U22" s="6" t="s">
         <v>79</v>
@@ -4436,50 +4442,50 @@
       </c>
       <c r="E23" s="2">
         <f ca="1">E24/(E26*(1-(E27-E28)))</f>
-        <v>0.19977610547016036</v>
+        <v>0.19235970565467586</v>
       </c>
       <c r="U23" s="6">
         <v>1</v>
       </c>
       <c r="V23" s="35">
         <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>21.989000000000001</v>
+        <v>21.945</v>
       </c>
       <c r="W23" s="36">
         <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>22.988500000000002</v>
+        <v>22.942500000000003</v>
       </c>
       <c r="X23" s="36">
         <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>23.988</v>
+        <v>23.94</v>
       </c>
       <c r="Y23" s="36">
         <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>24.987500000000001</v>
+        <v>24.9375</v>
       </c>
       <c r="Z23" s="36">
         <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>25.987000000000002</v>
+        <v>25.935000000000002</v>
       </c>
       <c r="AA23" s="36">
         <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>26.986500000000003</v>
+        <v>26.932500000000001</v>
       </c>
       <c r="AB23" s="36">
         <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>27.986000000000001</v>
+        <v>27.93</v>
       </c>
       <c r="AC23" s="36">
         <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>28.985500000000002</v>
+        <v>28.927500000000002</v>
       </c>
       <c r="AD23" s="36">
         <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>29.985000000000003</v>
+        <v>29.925000000000001</v>
       </c>
       <c r="AE23" s="36">
         <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U23-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>30.984500000000001</v>
+        <v>30.922500000000003</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.4">
@@ -4502,43 +4508,43 @@
       </c>
       <c r="V24" s="37">
         <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>21.990222222222222</v>
+        <v>21.951111111111111</v>
       </c>
       <c r="W24" s="38">
         <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>22.989777777777778</v>
+        <v>22.948888888888888</v>
       </c>
       <c r="X24" s="38">
         <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>23.989333333333335</v>
+        <v>23.946666666666665</v>
       </c>
       <c r="Y24" s="38">
         <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>24.988888888888887</v>
+        <v>24.944444444444443</v>
       </c>
       <c r="Z24" s="38">
         <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>25.988444444444443</v>
+        <v>25.94222222222222</v>
       </c>
       <c r="AA24" s="38">
         <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>26.988</v>
+        <v>26.94</v>
       </c>
       <c r="AB24" s="38">
         <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>27.987555555555556</v>
+        <v>27.937777777777779</v>
       </c>
       <c r="AC24" s="38">
         <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>28.987111111111112</v>
+        <v>28.935555555555556</v>
       </c>
       <c r="AD24" s="38">
         <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>29.986666666666665</v>
+        <v>29.933333333333334</v>
       </c>
       <c r="AE24" s="38">
         <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U24-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>30.986222222222221</v>
+        <v>30.931111111111111</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.4">
@@ -4560,43 +4566,43 @@
       </c>
       <c r="V25" s="37">
         <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>21.991444444444443</v>
+        <v>21.957222222222224</v>
       </c>
       <c r="W25" s="38">
         <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>22.991055555555555</v>
+        <v>22.955277777777777</v>
       </c>
       <c r="X25" s="38">
         <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>23.990666666666666</v>
+        <v>23.953333333333333</v>
       </c>
       <c r="Y25" s="38">
         <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>24.990277777777777</v>
+        <v>24.951388888888889</v>
       </c>
       <c r="Z25" s="38">
         <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>25.989888888888888</v>
+        <v>25.949444444444445</v>
       </c>
       <c r="AA25" s="38">
         <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>26.9895</v>
+        <v>26.947500000000002</v>
       </c>
       <c r="AB25" s="38">
         <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>27.989111111111111</v>
+        <v>27.945555555555558</v>
       </c>
       <c r="AC25" s="38">
         <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>28.988722222222222</v>
+        <v>28.94361111111111</v>
       </c>
       <c r="AD25" s="38">
         <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>29.988333333333333</v>
+        <v>29.941666666666666</v>
       </c>
       <c r="AE25" s="38">
         <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U25-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>30.987944444444445</v>
+        <v>30.939722222222223</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.4">
@@ -4605,7 +4611,7 @@
       </c>
       <c r="E26" s="4">
         <f ca="1">(E22-'Skill to Value'!C3)*(E25-D25)/('Skill to Value'!D3-'Skill to Value'!C3)+D25</f>
-        <v>27.54</v>
+        <v>28.64</v>
       </c>
       <c r="U26" s="6">
         <f t="shared" si="1"/>
@@ -4613,43 +4619,43 @@
       </c>
       <c r="V26" s="37">
         <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>21.992666666666668</v>
+        <v>21.963333333333331</v>
       </c>
       <c r="W26" s="38">
         <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>22.992333333333335</v>
+        <v>22.961666666666666</v>
       </c>
       <c r="X26" s="38">
         <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>23.992000000000001</v>
+        <v>23.96</v>
       </c>
       <c r="Y26" s="38">
         <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>24.991666666666667</v>
+        <v>24.958333333333332</v>
       </c>
       <c r="Z26" s="38">
         <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>25.991333333333333</v>
+        <v>25.956666666666667</v>
       </c>
       <c r="AA26" s="38">
         <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>26.991</v>
+        <v>26.954999999999998</v>
       </c>
       <c r="AB26" s="38">
         <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>27.990666666666669</v>
+        <v>27.953333333333333</v>
       </c>
       <c r="AC26" s="38">
         <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>28.990333333333336</v>
+        <v>28.951666666666664</v>
       </c>
       <c r="AD26" s="38">
         <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>29.990000000000002</v>
+        <v>29.95</v>
       </c>
       <c r="AE26" s="38">
         <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U26-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>30.989666666666668</v>
+        <v>30.948333333333331</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.4">
@@ -4661,7 +4667,7 @@
       </c>
       <c r="E27" s="4">
         <f>E14*((E16-'Skill to Value'!C3)*(D17-E17)/('Skill to Value'!D3-'Skill to Value'!C3)+E17)</f>
-        <v>3.333333333333337E-4</v>
+        <v>1.6666666666666685E-3</v>
       </c>
       <c r="U27" s="6">
         <f t="shared" si="1"/>
@@ -4669,43 +4675,43 @@
       </c>
       <c r="V27" s="37">
         <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>21.99388888888889</v>
+        <v>21.969444444444445</v>
       </c>
       <c r="W27" s="38">
         <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>22.993611111111111</v>
+        <v>22.968055555555555</v>
       </c>
       <c r="X27" s="38">
         <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>23.993333333333332</v>
+        <v>23.966666666666669</v>
       </c>
       <c r="Y27" s="38">
         <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>24.993055555555554</v>
+        <v>24.965277777777779</v>
       </c>
       <c r="Z27" s="38">
         <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>25.992777777777775</v>
+        <v>25.963888888888889</v>
       </c>
       <c r="AA27" s="38">
         <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>26.9925</v>
+        <v>26.962499999999999</v>
       </c>
       <c r="AB27" s="38">
         <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>27.992222222222221</v>
+        <v>27.961111111111112</v>
       </c>
       <c r="AC27" s="38">
         <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>28.991944444444442</v>
+        <v>28.959722222222222</v>
       </c>
       <c r="AD27" s="38">
         <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>29.991666666666667</v>
+        <v>29.958333333333332</v>
       </c>
       <c r="AE27" s="38">
         <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U27-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>30.991388888888888</v>
+        <v>30.956944444444446</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.4">
@@ -4731,43 +4737,43 @@
       </c>
       <c r="V28" s="37">
         <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>21.995111111111111</v>
+        <v>21.975555555555555</v>
       </c>
       <c r="W28" s="38">
         <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>22.994888888888887</v>
+        <v>22.974444444444444</v>
       </c>
       <c r="X28" s="38">
         <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>23.994666666666667</v>
+        <v>23.973333333333336</v>
       </c>
       <c r="Y28" s="38">
         <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>24.994444444444444</v>
+        <v>24.972222222222225</v>
       </c>
       <c r="Z28" s="38">
         <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>25.994222222222223</v>
+        <v>25.971111111111114</v>
       </c>
       <c r="AA28" s="38">
         <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>26.994</v>
+        <v>26.970000000000002</v>
       </c>
       <c r="AB28" s="38">
         <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>27.993777777777776</v>
+        <v>27.968888888888891</v>
       </c>
       <c r="AC28" s="38">
         <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>28.993555555555556</v>
+        <v>28.96777777777778</v>
       </c>
       <c r="AD28" s="38">
         <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>29.993333333333332</v>
+        <v>29.966666666666669</v>
       </c>
       <c r="AE28" s="38">
         <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U28-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>30.993111111111112</v>
+        <v>30.965555555555557</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.4">
@@ -4776,7 +4782,7 @@
       </c>
       <c r="E29" s="4">
         <f>(1-(E27-E28))</f>
-        <v>0.9996666666666667</v>
+        <v>0.99833333333333329</v>
       </c>
       <c r="U29" s="6">
         <f t="shared" si="1"/>
@@ -4784,43 +4790,43 @@
       </c>
       <c r="V29" s="37">
         <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>21.996333333333332</v>
+        <v>21.981666666666666</v>
       </c>
       <c r="W29" s="38">
         <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>22.996166666666667</v>
+        <v>22.980833333333333</v>
       </c>
       <c r="X29" s="38">
         <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>23.996000000000002</v>
+        <v>23.98</v>
       </c>
       <c r="Y29" s="38">
         <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>24.995833333333334</v>
+        <v>24.979166666666668</v>
       </c>
       <c r="Z29" s="38">
         <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>25.995666666666668</v>
+        <v>25.978333333333332</v>
       </c>
       <c r="AA29" s="38">
         <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>26.9955</v>
+        <v>26.977499999999999</v>
       </c>
       <c r="AB29" s="38">
         <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>27.995333333333335</v>
+        <v>27.976666666666667</v>
       </c>
       <c r="AC29" s="38">
         <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>28.995166666666666</v>
+        <v>28.975833333333334</v>
       </c>
       <c r="AD29" s="38">
         <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>29.995000000000001</v>
+        <v>29.974999999999998</v>
       </c>
       <c r="AE29" s="38">
         <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U29-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>30.994833333333332</v>
+        <v>30.974166666666665</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.4">
@@ -4829,7 +4835,7 @@
       </c>
       <c r="E30" s="25">
         <f ca="1">E26*E29</f>
-        <v>27.530819999999999</v>
+        <v>28.592266666666667</v>
       </c>
       <c r="U30" s="6">
         <f t="shared" si="1"/>
@@ -4837,43 +4843,43 @@
       </c>
       <c r="V30" s="37">
         <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>21.997555555555557</v>
+        <v>21.987777777777779</v>
       </c>
       <c r="W30" s="38">
         <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>22.997444444444447</v>
+        <v>22.987222222222222</v>
       </c>
       <c r="X30" s="38">
         <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>23.997333333333334</v>
+        <v>23.986666666666668</v>
       </c>
       <c r="Y30" s="38">
         <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>24.997222222222224</v>
+        <v>24.986111111111111</v>
       </c>
       <c r="Z30" s="38">
         <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>25.997111111111114</v>
+        <v>25.985555555555557</v>
       </c>
       <c r="AA30" s="38">
         <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>26.997</v>
+        <v>26.984999999999999</v>
       </c>
       <c r="AB30" s="38">
         <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>27.99688888888889</v>
+        <v>27.984444444444446</v>
       </c>
       <c r="AC30" s="38">
         <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>28.99677777777778</v>
+        <v>28.983888888888888</v>
       </c>
       <c r="AD30" s="38">
         <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>29.99666666666667</v>
+        <v>29.983333333333334</v>
       </c>
       <c r="AE30" s="38">
         <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U30-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>30.996555555555556</v>
+        <v>30.982777777777777</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.4">
@@ -4883,43 +4889,43 @@
       </c>
       <c r="V31" s="37">
         <f>((V$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>21.998777777777779</v>
+        <v>21.99388888888889</v>
       </c>
       <c r="W31" s="38">
         <f>((W$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>22.99872222222222</v>
+        <v>22.993611111111111</v>
       </c>
       <c r="X31" s="38">
         <f>((X$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>23.998666666666665</v>
+        <v>23.993333333333332</v>
       </c>
       <c r="Y31" s="38">
         <f>((Y$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>24.99861111111111</v>
+        <v>24.993055555555554</v>
       </c>
       <c r="Z31" s="38">
         <f>((Z$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>25.998555555555555</v>
+        <v>25.992777777777775</v>
       </c>
       <c r="AA31" s="38">
         <f>((AA$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>26.9985</v>
+        <v>26.9925</v>
       </c>
       <c r="AB31" s="38">
         <f>((AB$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>27.998444444444445</v>
+        <v>27.992222222222221</v>
       </c>
       <c r="AC31" s="38">
         <f>((AC$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>28.998388888888886</v>
+        <v>28.991944444444442</v>
       </c>
       <c r="AD31" s="38">
         <f>((AD$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>29.998333333333331</v>
+        <v>29.991666666666667</v>
       </c>
       <c r="AE31" s="38">
         <f>((AE$22-'Skill to Value'!$C$3)*($E$25-$D$25)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$25)*(1-($E$14*(($U31-'Skill to Value'!$C$3)*($E$17-$D$17)/('Skill to Value'!$D$3-'Skill to Value'!$C$3)+$D$17)-$E$28))</f>
-        <v>30.998277777777776</v>
+        <v>30.991388888888888</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.4">
@@ -4928,7 +4934,7 @@
       </c>
       <c r="E32" s="25">
         <f ca="1">E24/E23</f>
-        <v>27.530819999999999</v>
+        <v>28.592266666666667</v>
       </c>
       <c r="F32" t="s">
         <v>71</v>
@@ -4984,7 +4990,7 @@
       </c>
       <c r="E33" s="25">
         <f ca="1">E32*2.23694</f>
-        <v>61.584792490799998</v>
+        <v>63.959184997333338</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.4">
@@ -4993,7 +4999,7 @@
       </c>
       <c r="Y34" s="25">
         <f>Z27</f>
-        <v>25.992777777777775</v>
+        <v>25.963888888888889</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.4">
@@ -5869,6 +5875,16 @@
     <row r="90" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A90" s="39" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -5884,44 +5900,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId4" name="setPassAdjustment">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D28" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>119743</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>22</xdr:col>
-                <xdr:colOff>185057</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>59871</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1033" r:id="rId4" name="setPassAdjustment"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId6" name="distance">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D24" r:id="rId7">
+        <control shapeId="1026" r:id="rId4" name="timingVar">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
                 <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>9</xdr:row>
                 <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>23</xdr:col>
                 <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>9</xdr:row>
                 <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
@@ -5929,7 +5920,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId6" name="distance"/>
+        <control shapeId="1026" r:id="rId4" name="timingVar"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId6" name="SpikeSkill">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D16" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>20</xdr:col>
+                <xdr:colOff>108857</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>27214</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>23</xdr:col>
+                <xdr:colOff>397329</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>179614</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId6" name="SpikeSkill"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -5959,19 +5975,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId10" name="SpikeSkill">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D16" r:id="rId11">
+        <control shapeId="1030" r:id="rId10" name="distance">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D24" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
                 <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>11</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>27214</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>23</xdr:col>
                 <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>11</xdr:row>
+                <xdr:row>15</xdr:row>
                 <xdr:rowOff>179614</xdr:rowOff>
               </to>
             </anchor>
@@ -5979,32 +5995,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId10" name="SpikeSkill"/>
+        <control shapeId="1030" r:id="rId10" name="distance"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId12" name="timingVar">
-          <controlPr defaultSize="0" autoLine="0" linkedCell="D12" r:id="rId13">
+        <control shapeId="1033" r:id="rId12" name="setPassAdjustment">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="D28" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>20</xdr:col>
-                <xdr:colOff>108857</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>27214</xdr:rowOff>
+                <xdr:colOff>119743</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>23</xdr:col>
-                <xdr:colOff>397329</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
+                <xdr:col>22</xdr:col>
+                <xdr:colOff>185057</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>59871</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId12" name="timingVar"/>
+        <control shapeId="1033" r:id="rId12" name="setPassAdjustment"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>